<commit_message>
İş Takip Güncellemesi - 26.01.2026 13:59:41
</commit_message>
<xml_diff>
--- a/istakip.xlsx
+++ b/istakip.xlsx
@@ -826,7 +826,7 @@
         <v/>
       </c>
       <c r="L11" t="str">
-        <v>HERHANGİ BİRŞEY YAPILMADI</v>
+        <v>ÇALIŞMA ALANI İLANI YAPILDI</v>
       </c>
     </row>
     <row r="12">
@@ -864,7 +864,7 @@
         <v/>
       </c>
       <c r="L12" t="str">
-        <v>HERHANGİ BİRŞEY YAPILMADI</v>
+        <v>ÇALIŞMA ALANI İLANI YAPILDI</v>
       </c>
     </row>
     <row r="13">
@@ -902,7 +902,7 @@
         <v/>
       </c>
       <c r="L13" t="str">
-        <v>HERHANGİ BİRŞEY YAPILMADI</v>
+        <v>ÇALIŞMA ALANI İLANI YAPILDI</v>
       </c>
     </row>
     <row r="14">
@@ -940,7 +940,7 @@
         <v/>
       </c>
       <c r="L14" t="str">
-        <v>HERHANGİ BİRŞEY YAPILMADI</v>
+        <v>ÇALIŞMA ALANI İLANI YAPILDI</v>
       </c>
     </row>
     <row r="15">
@@ -978,7 +978,7 @@
         <v/>
       </c>
       <c r="L15" t="str">
-        <v>HERHANGİ BİRŞEY YAPILMADI</v>
+        <v>ÇALIŞMA ALANI İLANI YAPILDI</v>
       </c>
     </row>
     <row r="16">
@@ -1016,7 +1016,7 @@
         <v/>
       </c>
       <c r="L16" t="str">
-        <v>HERHANGİ BİRŞEY YAPILMADI</v>
+        <v>ÇALIŞMA ALANI İLANI YAPILDI</v>
       </c>
     </row>
     <row r="17">
@@ -1054,7 +1054,7 @@
         <v/>
       </c>
       <c r="L17" t="str">
-        <v>HERHANGİ BİRŞEY YAPILMADI</v>
+        <v>ÇALIŞMA ALANI İLANI YAPILDI</v>
       </c>
     </row>
     <row r="18">
@@ -1092,7 +1092,7 @@
         <v/>
       </c>
       <c r="L18" t="str">
-        <v>HERHANGİ BİRŞEY YAPILMADI</v>
+        <v>ÇALIŞMA ALANI İLANI YAPILDI</v>
       </c>
     </row>
     <row r="19">
@@ -1130,7 +1130,7 @@
         <v/>
       </c>
       <c r="L19" t="str">
-        <v>HERHANGİ BİRŞEY YAPILMADI</v>
+        <v>ÇALIŞMA ALANI İLANI YAPILDI</v>
       </c>
     </row>
     <row r="20">
@@ -1168,7 +1168,7 @@
         <v/>
       </c>
       <c r="L20" t="str">
-        <v>HERHANGİ BİRŞEY YAPILMADI</v>
+        <v>ÇALIŞMA ALANI İLANI YAPILDI</v>
       </c>
     </row>
     <row r="21">
@@ -1206,7 +1206,7 @@
         <v/>
       </c>
       <c r="L21" t="str">
-        <v>HERHANGİ BİRŞEY YAPILMADI</v>
+        <v>ÇALIŞMA ALANI İLANI YAPILDI</v>
       </c>
     </row>
     <row r="22">
@@ -1244,7 +1244,7 @@
         <v/>
       </c>
       <c r="L22" t="str">
-        <v>HERHANGİ BİRŞEY YAPILMADI</v>
+        <v>ÇALIŞMA ALANI İLANI YAPILDI</v>
       </c>
     </row>
     <row r="23">
@@ -1282,7 +1282,7 @@
         <v/>
       </c>
       <c r="L23" t="str">
-        <v>HERHANGİ BİRŞEY YAPILMADI</v>
+        <v>ÇALIŞMA ALANI İLANI YAPILDI</v>
       </c>
     </row>
     <row r="24">
@@ -1320,7 +1320,7 @@
         <v/>
       </c>
       <c r="L24" t="str">
-        <v>HERHANGİ BİRŞEY YAPILMADI</v>
+        <v>ÇALIŞMA ALANI İLANI YAPILDI</v>
       </c>
     </row>
     <row r="25">
@@ -1358,7 +1358,7 @@
         <v/>
       </c>
       <c r="L25" t="str">
-        <v>HERHANGİ BİRŞEY YAPILMADI</v>
+        <v>ÇALIŞMA ALANI İLANI YAPILDI</v>
       </c>
     </row>
     <row r="26">
@@ -1396,7 +1396,7 @@
         <v/>
       </c>
       <c r="L26" t="str">
-        <v>HERHANGİ BİRŞEY YAPILMADI</v>
+        <v>ÇALIŞMA ALANI İLANI YAPILDI</v>
       </c>
     </row>
     <row r="27">
@@ -1434,7 +1434,7 @@
         <v/>
       </c>
       <c r="L27" t="str">
-        <v>HERHANGİ BİRŞEY YAPILMADI</v>
+        <v>ÇALIŞMA ALANI İLANI YAPILDI</v>
       </c>
     </row>
     <row r="28">
@@ -1472,7 +1472,7 @@
         <v/>
       </c>
       <c r="L28" t="str">
-        <v>HERHANGİ BİRŞEY YAPILMADI</v>
+        <v>ÇALIŞMA ALANI İLANI YAPILDI</v>
       </c>
     </row>
     <row r="29">
@@ -1510,7 +1510,7 @@
         <v/>
       </c>
       <c r="L29" t="str">
-        <v>HERHANGİ BİRŞEY YAPILMADI</v>
+        <v>ÇALIŞMA ALANI İLANI YAPILDI</v>
       </c>
     </row>
     <row r="30">
@@ -1548,7 +1548,7 @@
         <v/>
       </c>
       <c r="L30" t="str">
-        <v>HERHANGİ BİRŞEY YAPILMADI</v>
+        <v>ÇALIŞMA ALANI İLANI YAPILDI</v>
       </c>
     </row>
     <row r="31">
@@ -1586,7 +1586,7 @@
         <v/>
       </c>
       <c r="L31" t="str">
-        <v>HERHANGİ BİRŞEY YAPILMADI</v>
+        <v>ÇALIŞMA ALANI İLANI YAPILDI</v>
       </c>
     </row>
     <row r="32">
@@ -1624,7 +1624,7 @@
         <v/>
       </c>
       <c r="L32" t="str">
-        <v>HERHANGİ BİRŞEY YAPILMADI</v>
+        <v>ÇALIŞMA ALANI İLANI YAPILDI</v>
       </c>
     </row>
     <row r="33">

</xml_diff>

<commit_message>
İş Takip Güncellemesi - 26.01.2026 14:00:14
</commit_message>
<xml_diff>
--- a/istakip.xlsx
+++ b/istakip.xlsx
@@ -2612,7 +2612,7 @@
         <v>2025-10-31</v>
       </c>
       <c r="L58" t="str">
-        <v>DEĞERLENDİRMEDE</v>
+        <v>ASKI İLANINA HAZIRLANIYOR</v>
       </c>
     </row>
     <row r="59">
@@ -2726,7 +2726,7 @@
         <v>2025-10-31</v>
       </c>
       <c r="L61" t="str">
-        <v>DEĞERLENDİRMEDE</v>
+        <v>ASKI İLANINA HAZIRLANIYOR</v>
       </c>
     </row>
     <row r="62">
@@ -2802,7 +2802,7 @@
         <v>2025-10-31</v>
       </c>
       <c r="L63" t="str">
-        <v>DEĞERLENDİRMEDE</v>
+        <v>ASKI İLANINA HAZIRLANIYOR</v>
       </c>
     </row>
     <row r="64">
@@ -3989,7 +3989,7 @@
         <v>2025-10-31</v>
       </c>
       <c r="L94" t="str">
-        <v>DEĞERLENDİRMEDE</v>
+        <v>ASKI İLANINA HAZIRLANIYOR</v>
       </c>
     </row>
     <row r="95">

</xml_diff>

<commit_message>
İş Takip Güncellemesi - 30.01.2026 11:48:17
</commit_message>
<xml_diff>
--- a/istakip.xlsx
+++ b/istakip.xlsx
@@ -826,7 +826,7 @@
         <v/>
       </c>
       <c r="L11" t="str">
-        <v>ÇALIŞMA ALANI İLANI YAPILDI</v>
+        <v>ARAZİ DEVAM EDİYOR</v>
       </c>
     </row>
     <row r="12">
@@ -1396,7 +1396,7 @@
         <v/>
       </c>
       <c r="L26" t="str">
-        <v>ÇALIŞMA ALANI İLANI YAPILDI</v>
+        <v>ARAZİ DEVAM EDİYOR</v>
       </c>
     </row>
     <row r="27">
@@ -1472,7 +1472,7 @@
         <v/>
       </c>
       <c r="L28" t="str">
-        <v>ÇALIŞMA ALANI İLANI YAPILDI</v>
+        <v>ARAZİ DEVAM EDİYOR</v>
       </c>
     </row>
     <row r="29">

</xml_diff>

<commit_message>
İş Takip Güncellemesi - 30.01.2026 11:49:12
</commit_message>
<xml_diff>
--- a/istakip.xlsx
+++ b/istakip.xlsx
@@ -864,7 +864,7 @@
         <v/>
       </c>
       <c r="L12" t="str">
-        <v>ÇALIŞMA ALANI İLANI YAPILDI</v>
+        <v>ARAZİ DEVAM EDİYOR</v>
       </c>
     </row>
     <row r="13">
@@ -1472,7 +1472,7 @@
         <v/>
       </c>
       <c r="L28" t="str">
-        <v>ARAZİ DEVAM EDİYOR</v>
+        <v>ÇALIŞMA ALANI İLANI YAPILDI</v>
       </c>
     </row>
     <row r="29">

</xml_diff>

<commit_message>
İş Takip Güncellemesi - 02.02.2026 13:30:30
</commit_message>
<xml_diff>
--- a/istakip.xlsx
+++ b/istakip.xlsx
@@ -5,11 +5,10 @@
   <sheets>
     <sheet name="İş Takip Listesi" sheetId="1" r:id="rId1"/>
     <sheet name="Güncelleme" sheetId="2" r:id="rId2"/>
-    <sheet name="Güncelleme(2026)" sheetId="3" r:id="rId3"/>
-    <sheet name="Personel" sheetId="4" r:id="rId4"/>
-    <sheet name="İlçe" sheetId="5" r:id="rId5"/>
-    <sheet name="Uygulama" sheetId="6" r:id="rId6"/>
-    <sheet name="Liste" sheetId="7" r:id="rId7"/>
+    <sheet name="Personel" sheetId="3" r:id="rId3"/>
+    <sheet name="İlçe" sheetId="4" r:id="rId4"/>
+    <sheet name="Uygulama" sheetId="5" r:id="rId5"/>
+    <sheet name="Liste" sheetId="6" r:id="rId6"/>
   </sheets>
 </workbook>
 </file>
@@ -4320,27 +4319,18 @@
         <v>FİRMAYA TESLİM EDİLDİ</v>
       </c>
       <c r="M102" t="str" xml:space="preserve">
-        <v xml:space="preserve">01.11.2025 firmaya teslim edilecek_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-07.11.2025 ormanı bakıp teslim edecek_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-10.11.2025 kontrol edilip firmaya teslim edilecek_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-10.11.2025 Ormancı 11.11.2025 teslim edecek_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-13.11.2025 Ormancı 17.11.2025 teslim edecek_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-20.11.2025 orman mükerrerliği ile ilgili beyanname düzenlendi tescili bekleniyor_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-02.12.2025 Krokilerine başlanıldı_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-15.12.2025 Proje hazırlanıyor_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-22.12.2025 Proje hazırlanıyor _x000d__x000d__x000d_
-_x000d__x000d__x000d_
-05.01.2026 KROKİLERE BAŞLANACAK_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-15.01.2026 Devam ediyor firma</v>
+        <v xml:space="preserve">01.11.2025 firmaya teslim edilecek
+07.11.2025 ormanı bakıp teslim edecek
+10.11.2025 kontrol edilip firmaya teslim edilecek
+10.11.2025 Ormancı 11.11.2025 teslim edecek
+13.11.2025 Ormancı 17.11.2025 teslim edecek
+20.11.2025 orman mükerrerliği ile ilgili beyanname düzenlendi tescili bekleniyor
+02.12.2025 Krokilerine başlanıldı
+15.12.2025 Proje hazırlanıyor
+22.12.2025 Proje hazırlanıyor 
+05.01.2026 KROKİLERE BAŞLANACAK
+15.01.2026 Devam ediyor firma
+31.01.2026 Personel kontrolünde 09-13.02 askı ilanı yapılacak</v>
       </c>
     </row>
     <row r="103">
@@ -4498,23 +4488,16 @@
         <v>KROKİ/TUTANAK KONTROLÜ</v>
       </c>
       <c r="M106" t="str" xml:space="preserve">
-        <v xml:space="preserve">03.11.2025 firmaya teslim edilecek_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-05.11.2025 kontroller devam ediyor 10.11.2025 bazı yerlerin arazi kontrolleri yapılacak_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-13.11.2025 arazi kontrolü 18.11.2025 de yapılıp, 21.11.2025 de firmaya teslim edilecek_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-20.11.2025 arazi kontrolü yapılıyor 24.11.2025 de firmaya teslim edilecek_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-02.12.2025 krokileri hazırlanıyor_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-15.12.2025 Krokileri basılıyor_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-22.12.2025 Kroki kontrolü 25.12.2025 biticek_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-02.01.2026 Tutanaklarına başlanıldı_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-15.01.2026 TEMUR beyin kontrolünde</v>
+        <v xml:space="preserve">03.11.2025 firmaya teslim edilecek
+05.11.2025 kontroller devam ediyor 10.11.2025 bazı yerlerin arazi kontrolleri yapılacak
+13.11.2025 arazi kontrolü 18.11.2025 de yapılıp, 21.11.2025 de firmaya teslim edilecek
+20.11.2025 arazi kontrolü yapılıyor 24.11.2025 de firmaya teslim edilecek
+02.12.2025 krokileri hazırlanıyor
+15.12.2025 Krokileri basılıyor
+22.12.2025 Kroki kontrolü 25.12.2025 biticek
+02.01.2026 Tutanaklarına başlanıldı
+15.01.2026 TEMUR beyin kontrolünde
+31.01.2026 03.02 askı yapılacak</v>
       </c>
     </row>
     <row r="107" xml:space="preserve">
@@ -4727,22 +4710,16 @@
         <v>ASKI İLANINA HAZIRLANIYOR</v>
       </c>
       <c r="M111" t="str" xml:space="preserve">
-        <v xml:space="preserve">24.10.2025 firmaya teslim edilecek_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-28.10.2025 firmaya teslim edilecek_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-03.11.2025 ormancı kontrolünde_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-20.11.2025 ormancı kontrolünde_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-02.12.2025 Firmaya teslim edildi_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-15.12.2025 Proje hazırlanıyor_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-22.12.2025 Kroki hazırlanıyor. 26.12.205 de biticek_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-02.01.2026 Kroki kontrolüne 05.01.2026 başlanıp 08.01.2026 bitip tutanağa geçilecek _x000d__x000d__x000d_
-15.01.2026 Tutanak başlanılacak</v>
+        <v xml:space="preserve">24.10.2025 firmaya teslim edilecek
+28.10.2025 firmaya teslim edilecek
+03.11.2025 ormancı kontrolünde
+20.11.2025 ormancı kontrolünde
+02.12.2025 Firmaya teslim edildi
+15.12.2025 Proje hazırlanıyor
+22.12.2025 Kroki hazırlanıyor. 26.12.205 de biticek
+02.01.2026 Kroki kontrolüne 05.01.2026 başlanıp 08.01.2026 bitip tutanağa geçilecek 
+15.01.2026 Tutanak başlanılacak
+31.01.2026 imza aşamasında haftaiçi askı yapılacak</v>
       </c>
     </row>
     <row r="112">
@@ -4870,15 +4847,12 @@
         <v>KROKİ/TUTANAK KONTROLÜ</v>
       </c>
       <c r="M114" t="str" xml:space="preserve">
-        <v xml:space="preserve">14.11.2025 firmaya teslim edilecek_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-02.12.2025 araziye çıkılacak_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-15.12.2025 Kısmi arazi kontrolü yapılıp firmaya teslim edilecek(22.12.2025)_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-02.01.2026 Firmaya 05.01.2026 teslim edilecek_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-15.01.2026 Kroki kontrolünde</v>
+        <v xml:space="preserve">14.11.2025 firmaya teslim edilecek
+02.12.2025 araziye çıkılacak
+15.12.2025 Kısmi arazi kontrolü yapılıp firmaya teslim edilecek(22.12.2025)
+02.01.2026 Firmaya 05.01.2026 teslim edilecek
+15.01.2026 Kroki kontrolünde
+31.01.2026 Kroki müh. kontrolünde</v>
       </c>
     </row>
     <row r="115" xml:space="preserve">
@@ -4919,13 +4893,14 @@
         <v>DEĞERLENDİRMEDE</v>
       </c>
       <c r="M115" t="str" xml:space="preserve">
-        <v xml:space="preserve">Kıymetlendirmede eksiklikler var firma tamamlayacak bu hafta(20.10.2025)_x000d__x000d__x000d__x000d__x000d_
-05.11.2025 eksik uçuşlar teslim edildi_x000d__x000d__x000d__x000d__x000d_
-10.11.2025 kıymetlendirmeler kontrol ediliyor_x000d__x000d__x000d__x000d__x000d_
-13.11.2025 Firmaya 28.11.2025 de teslim edilecek_x000d__x000d__x000d__x000d__x000d_
-15.12.2025 Değerlendirme devam ediyor_x000d__x000d__x000d__x000d__x000d_
-22.12.2025 Kısmi uçuş yapıldı kıymetlendirme yapılıyor aynı zamanda değerlendirme devam ediyor_x000d__x000d__x000d__x000d__x000d_
-02.01.2026 Değerlendirme 15.01.2026 biticek</v>
+        <v xml:space="preserve">Kıymetlendirmede eksiklikler var firma tamamlayacak bu hafta(20.10.2025)
+05.11.2025 eksik uçuşlar teslim edildi
+10.11.2025 kıymetlendirmeler kontrol ediliyor
+13.11.2025 Firmaya 28.11.2025 de teslim edilecek
+15.12.2025 Değerlendirme devam ediyor
+22.12.2025 Kısmi uçuş yapıldı kıymetlendirme yapılıyor aynı zamanda değerlendirme devam ediyor
+02.01.2026 Değerlendirme 15.01.2026 biticek
+31.01.2026 firma projeyi hazırlıyor 16.02.2026 tamamlayacak</v>
       </c>
     </row>
     <row r="116" xml:space="preserve">
@@ -4966,12 +4941,13 @@
         <v>FİRMAYA TESLİM EDİLDİ</v>
       </c>
       <c r="M116" t="str" xml:space="preserve">
-        <v xml:space="preserve">01.11.2025 firmaya teslim edilecek_x000d__x000d__x000d__x000d__x000d_
-05.11.2025 kontroller devam ediyor_x000d__x000d__x000d__x000d__x000d_
-13.11.2025 Firmaya 28.11.2025 teslim edilecek_x000d__x000d__x000d__x000d__x000d_
-02.12.2025 Firmaya 05.12.2025 teslim edilecek_x000d__x000d__x000d__x000d__x000d_
-15.12.2025 Değerlendirme devam ediyor_x000d__x000d__x000d__x000d__x000d_
-02.01.2026 Firmaya 15.01.2026 Teslim edilecek</v>
+        <v xml:space="preserve">01.11.2025 firmaya teslim edilecek
+05.11.2025 kontroller devam ediyor
+13.11.2025 Firmaya 28.11.2025 teslim edilecek
+02.12.2025 Firmaya 05.12.2025 teslim edilecek
+15.12.2025 Değerlendirme devam ediyor
+02.01.2026 Firmaya 15.01.2026 Teslim edilecek
+31.01.2026 firma projeyi hazırlıyor 16.02.2026 tamamlayacak</v>
       </c>
     </row>
     <row r="117" xml:space="preserve">
@@ -5012,23 +4988,16 @@
         <v>KROKİ/TUTANAK KONTROLÜ</v>
       </c>
       <c r="M117" t="str" xml:space="preserve">
-        <v xml:space="preserve">01.11.2025 firmaya teslim edilecek_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-07.11.2025 firmaya teslim edilecek_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-10.11.2025 Firmaya 12.11.2025 de teslim edilecek_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-13.11.2025 Firmaya 14.11.2025 de teslim edilecek_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-20.11.2025 krokilere 22.11.2025 de başlanarak 24.11.2025 kontrol için verilecek_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-02.12.2025 Krokiler hazırlanıp kontrolleri yapılıyor_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-15.12.2025 Kroki kontrolü devam ediyor_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-22.12.2025 krokiler 24.12.2025 de bitecek_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-15.01.2026 Tutanak kontrolü devam ediyor</v>
+        <v xml:space="preserve">01.11.2025 firmaya teslim edilecek
+07.11.2025 firmaya teslim edilecek
+10.11.2025 Firmaya 12.11.2025 de teslim edilecek
+13.11.2025 Firmaya 14.11.2025 de teslim edilecek
+20.11.2025 krokilere 22.11.2025 de başlanarak 24.11.2025 kontrol için verilecek
+02.12.2025 Krokiler hazırlanıp kontrolleri yapılıyor
+15.12.2025 Kroki kontrolü devam ediyor
+22.12.2025 krokiler 24.12.2025 de bitecek
+15.01.2026 Tutanak kontrolü devam ediyor
+31.01.2026 09-13.02 askı ilanı yapılacak</v>
       </c>
     </row>
     <row r="118" xml:space="preserve">
@@ -5128,9 +5097,9 @@
         <v>DEĞERLENDİRMEDE</v>
       </c>
       <c r="M119" t="str" xml:space="preserve">
-        <v xml:space="preserve">15.12.2025 Değerlendirme devam ediyor_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-22.12.2025 Arazi uçuş yapılacak yerler var. Değerlendirme devam ediyor.</v>
+        <v xml:space="preserve">15.12.2025 Değerlendirme devam ediyor
+22.12.2025 Arazi uçuş yapılacak yerler var. Değerlendirme devam ediyor.
+31.01.2026 Haftaiçi ormancı ve arazi kontrolü sonrası haftasonu firma kroki çalışmalarına başlayacak</v>
       </c>
     </row>
     <row r="120" xml:space="preserve">
@@ -12216,67 +12185,6 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>İLÇE</v>
-      </c>
-      <c r="B1" t="str">
-        <v>BİRİM</v>
-      </c>
-      <c r="C1" t="str">
-        <v>PARSEL SAYISI</v>
-      </c>
-      <c r="D1" t="str">
-        <v>İDÖ PARSEL SAYISI</v>
-      </c>
-      <c r="E1" t="str">
-        <v>TOPLAM PARSEL</v>
-      </c>
-      <c r="F1" t="str">
-        <v>İŞE BAŞLAMA</v>
-      </c>
-      <c r="G1" t="str">
-        <v>BİTİŞ TARİHİ</v>
-      </c>
-      <c r="H1" t="str">
-        <v>ARAZİ YERSEL ÖLÇÜM TARİHİ(YAPILAN)</v>
-      </c>
-      <c r="I1" t="str">
-        <v>UÇUŞ TARİHİ(YAPILAN)</v>
-      </c>
-      <c r="J1" t="str">
-        <v>UÇUŞ KIYMETLENDİRME DURUM</v>
-      </c>
-      <c r="K1" t="str">
-        <v>DEĞERLENDİRME DURUM</v>
-      </c>
-      <c r="L1" t="str">
-        <v>ORMAN ASKI TARİHİ</v>
-      </c>
-      <c r="M1" t="str">
-        <v>BİLGİLENDİRME İLANI TARİHİ</v>
-      </c>
-      <c r="N1" t="str">
-        <v>KOMİSYON DURUM</v>
-      </c>
-      <c r="O1" t="str">
-        <v>KESİN ASKI TARİHİ</v>
-      </c>
-    </row>
-  </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:O1"/>
-  </ignoredErrors>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B76"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -12897,7 +12805,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A14"/>
   <sheetViews>
@@ -12981,7 +12889,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A6"/>
   <sheetViews>
@@ -13025,7 +12933,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D26"/>
   <sheetViews>

</xml_diff>

<commit_message>
İş Takip Güncellemesi - 02.02.2026 13:35:04
</commit_message>
<xml_diff>
--- a/istakip.xlsx
+++ b/istakip.xlsx
@@ -4143,8 +4143,9 @@
         <v>FİRMAYA TESLİM EDİLDİ</v>
       </c>
       <c r="M98" t="str" xml:space="preserve">
-        <v xml:space="preserve">Ormancı kontrolünde(13.10.2025)_x000d__x000d__x000d__x000d__x000d_
-GM OLUR'u beklenecek</v>
+        <v xml:space="preserve">Ormancı kontrolünde(13.10.2025)
+GM OLUR'u beklenecek
+31.01.2026 kroki basılıyor</v>
       </c>
     </row>
     <row r="99">
@@ -5038,24 +5039,16 @@
         <v>FİRMAYA TESLİM EDİLDİ</v>
       </c>
       <c r="M118" t="str" xml:space="preserve">
-        <v xml:space="preserve">01.11.2025 firmaya teslim edilecek_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-05.11.2025 kontroller devam ediyor_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-10.11.2025 Değerlendrime 13.11.2025 de bitecek_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-13.11.2025 Firmaya 17-21 haftası teslim edilecek_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-20.11.2025 firmaya 24.11.2025 de teslim edilecek_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-02.12.2025 bugün firmaya teslim edilecek_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-15.12.2025 Proje hazırlanıyor_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-22.12.2025 Proje 25.12.2025 biticek, krokiler 30.12.2025 verilecek_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-02.01.2026 Firma projeyi hazırlıyor _x000d__x000d__x000d_
-_x000d__x000d__x000d_
+        <v xml:space="preserve">01.11.2025 firmaya teslim edilecek
+05.11.2025 kontroller devam ediyor
+31.01.2026 firma kroki hazırlıyor
+10.11.2025 Değerlendrime 13.11.2025 de bitecek
+13.11.2025 Firmaya 17-21 haftası teslim edilecek
+20.11.2025 firmaya 24.11.2025 de teslim edilecek
+02.12.2025 bugün firmaya teslim edilecek
+15.12.2025 Proje hazırlanıyor
+22.12.2025 Proje 25.12.2025 biticek, krokiler 30.12.2025 verilecek
+02.01.2026 Firma projeyi hazırlıyor 
 15.01.2026 kroki hazırlanıyor</v>
       </c>
     </row>

</xml_diff>

<commit_message>
İş Takip Güncellemesi - 03.02.2026 09:18:03
</commit_message>
<xml_diff>
--- a/istakip.xlsx
+++ b/istakip.xlsx
@@ -4486,7 +4486,7 @@
         <v>2025-05-23</v>
       </c>
       <c r="L106" t="str">
-        <v>KROKİ/TUTANAK KONTROLÜ</v>
+        <v>BİLGİLENDİRME İLANINDA</v>
       </c>
       <c r="M106" t="str" xml:space="preserve">
         <v xml:space="preserve">03.11.2025 firmaya teslim edilecek
@@ -8870,7 +8870,7 @@
         <v/>
       </c>
       <c r="M13" t="str">
-        <v/>
+        <v>2026-02-04</v>
       </c>
       <c r="N13" t="str">
         <v/>

</xml_diff>

<commit_message>
İş Takip Güncellemesi - 03.02.2026 09:19:06
</commit_message>
<xml_diff>
--- a/istakip.xlsx
+++ b/istakip.xlsx
@@ -9202,10 +9202,10 @@
         <v>2025-12-23</v>
       </c>
       <c r="N20" t="str">
-        <v/>
+        <v>Yapıldı</v>
       </c>
       <c r="O20" t="str">
-        <v/>
+        <v>2026-02-04</v>
       </c>
     </row>
     <row r="21">

</xml_diff>

<commit_message>
İş Takip Güncellemesi - 03.02.2026 09:19:57
</commit_message>
<xml_diff>
--- a/istakip.xlsx
+++ b/istakip.xlsx
@@ -4758,7 +4758,7 @@
         <v>2025-05-23</v>
       </c>
       <c r="L112" t="str">
-        <v>BİLGİLENDİRME İLANINDA</v>
+        <v>KESİN ASKIDA</v>
       </c>
       <c r="M112" t="str">
         <v>[x] 20.10.2025 askıya çıkacak</v>
@@ -9155,10 +9155,10 @@
         <v>2025-10-27</v>
       </c>
       <c r="N19" t="str">
-        <v/>
+        <v>Yapıldı</v>
       </c>
       <c r="O19" t="str">
-        <v/>
+        <v>2026-02-04</v>
       </c>
     </row>
     <row r="20">

</xml_diff>

<commit_message>
İş Takip Güncellemesi - 05.02.2026 15:01:46
</commit_message>
<xml_diff>
--- a/istakip.xlsx
+++ b/istakip.xlsx
@@ -4150,7 +4150,7 @@
     </row>
     <row r="99">
       <c r="A99" t="str">
-        <v>HAYIR</v>
+        <v>EVET</v>
       </c>
       <c r="B99" t="str">
         <v>Toroslar</v>
@@ -4369,12 +4369,12 @@
         <v>2025-05-23</v>
       </c>
       <c r="L103" t="str">
-        <v>KESİN ASKIDA</v>
+        <v>KESİN ASKIDAN İNDİ. BEKLEMEDE</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="str">
-        <v>HAYIR</v>
+        <v>EVET</v>
       </c>
       <c r="B104" t="str">
         <v>Toroslar</v>
@@ -4445,7 +4445,7 @@
         <v>2025-05-23</v>
       </c>
       <c r="L105" t="str">
-        <v>KESİN ASKIDA</v>
+        <v>KESİN ASKIDAN İNDİ. BEKLEMEDE</v>
       </c>
       <c r="M105" t="str">
         <v>[x] 21.10.2025 komisyon yapılacak(İsmail Pehlivan)</v>
@@ -4582,7 +4582,7 @@
         <v>2025-05-23</v>
       </c>
       <c r="L108" t="str">
-        <v>KESİN ASKIDA</v>
+        <v>KESİN ASKIDAN İNDİ. BEKLEMEDE</v>
       </c>
       <c r="M108" t="str">
         <v>[x] 21.10.2025 komisyon yapılacak(Lokman)</v>

</xml_diff>

<commit_message>
İş Takip Güncellemesi - 06.02.2026 14:00:39
</commit_message>
<xml_diff>
--- a/istakip.xlsx
+++ b/istakip.xlsx
@@ -4150,7 +4150,7 @@
     </row>
     <row r="99">
       <c r="A99" t="str">
-        <v>HAYIR</v>
+        <v>EVET</v>
       </c>
       <c r="B99" t="str">
         <v>Toroslar</v>
@@ -4183,7 +4183,7 @@
         <v>2025-05-23</v>
       </c>
       <c r="L99" t="str">
-        <v>KESİN ASKIDA</v>
+        <v>KESİN ASKIDAN İNDİ. BEKLEMEDE</v>
       </c>
     </row>
     <row r="100" xml:space="preserve">

</xml_diff>

<commit_message>
İş Takip Güncellemesi - 10.02.2026 12:17:16
</commit_message>
<xml_diff>
--- a/istakip.xlsx
+++ b/istakip.xlsx
@@ -825,7 +825,7 @@
         <v/>
       </c>
       <c r="L11" t="str">
-        <v>ARAZİ DEVAM EDİYOR</v>
+        <v>ÇALIŞMA ALANI İLANI YAPILDI</v>
       </c>
     </row>
     <row r="12">
@@ -863,7 +863,7 @@
         <v/>
       </c>
       <c r="L12" t="str">
-        <v>ARAZİ DEVAM EDİYOR</v>
+        <v>KROKİ/TUTANAK KONTROLÜ</v>
       </c>
     </row>
     <row r="13">
@@ -1395,7 +1395,7 @@
         <v/>
       </c>
       <c r="L26" t="str">
-        <v>ARAZİ DEVAM EDİYOR</v>
+        <v>KROKİ/TUTANAK KONTROLÜ</v>
       </c>
     </row>
     <row r="27">
@@ -1471,7 +1471,7 @@
         <v/>
       </c>
       <c r="L28" t="str">
-        <v>ARAZİ DEVAM EDİYOR</v>
+        <v>KROKİ/TUTANAK KONTROLÜ</v>
       </c>
     </row>
     <row r="29">

</xml_diff>

<commit_message>
İş Takip Güncellemesi - 10.02.2026 12:40:32
</commit_message>
<xml_diff>
--- a/istakip.xlsx
+++ b/istakip.xlsx
@@ -1015,7 +1015,10 @@
         <v/>
       </c>
       <c r="L16" t="str">
-        <v>ÇALIŞMA ALANI İLANI YAPILDI</v>
+        <v>ARAZİ DEVAM EDİYOR</v>
+      </c>
+      <c r="M16" t="str">
+        <v>10.02.2026 Araziye 12.02 de gidilecek</v>
       </c>
     </row>
     <row r="17">
@@ -1053,7 +1056,7 @@
         <v/>
       </c>
       <c r="L17" t="str">
-        <v>ÇALIŞMA ALANI İLANI YAPILDI</v>
+        <v>ARAZİ DEVAM EDİYOR</v>
       </c>
       <c r="M17" t="str">
         <v>10.02.2026 Araziye 11.02 de gidilecek</v>

</xml_diff>

<commit_message>
İş Takip Güncellemesi - 11.02.2026 12:41:41
</commit_message>
<xml_diff>
--- a/istakip.xlsx
+++ b/istakip.xlsx
@@ -4714,7 +4714,7 @@
         <v>2025-05-23</v>
       </c>
       <c r="L111" t="str">
-        <v>ASKI İLANINA HAZIRLANIYOR</v>
+        <v>BİLGİLENDİRME İLANINDA</v>
       </c>
       <c r="M111" t="str" xml:space="preserve">
         <v xml:space="preserve">24.10.2025 firmaya teslim edilecek_x000d_
@@ -9333,13 +9333,13 @@
         <v>Yapıldı</v>
       </c>
       <c r="K18" t="str">
-        <v>Firmaya Teslim Edildi</v>
+        <v>Yapıldı</v>
       </c>
       <c r="L18" t="str">
         <v/>
       </c>
       <c r="M18" t="str">
-        <v/>
+        <v>2026-02-12</v>
       </c>
       <c r="N18" t="str">
         <v/>

</xml_diff>

<commit_message>
İş Takip Güncellemesi - 11.02.2026 13:57:33
</commit_message>
<xml_diff>
--- a/istakip.xlsx
+++ b/istakip.xlsx
@@ -4323,7 +4323,7 @@
         <v>2025-05-23</v>
       </c>
       <c r="L102" t="str">
-        <v>FİRMAYA TESLİM EDİLDİ</v>
+        <v>KROKİ/TUTANAK KONTROLÜ</v>
       </c>
       <c r="M102" t="str" xml:space="preserve">
         <v xml:space="preserve">01.11.2025 firmaya teslim edilecek_x000d_
@@ -4851,15 +4851,16 @@
         <v>2025-05-23</v>
       </c>
       <c r="L114" t="str">
-        <v>KROKİ/TUTANAK KONTROLÜ</v>
+        <v>ASKI İLANINA HAZIRLANIYOR</v>
       </c>
       <c r="M114" t="str" xml:space="preserve">
-        <v xml:space="preserve">14.11.2025 firmaya teslim edilecek_x000d_
-02.12.2025 araziye çıkılacak_x000d_
-15.12.2025 Kısmi arazi kontrolü yapılıp firmaya teslim edilecek(22.12.2025)_x000d_
-02.01.2026 Firmaya 05.01.2026 teslim edilecek_x000d_
-15.01.2026 Kroki kontrolünde_x000d_
-31.01.2026 Kroki müh. kontrolünde</v>
+        <v xml:space="preserve">14.11.2025 firmaya teslim edilecek
+02.12.2025 araziye çıkılacak
+15.12.2025 Kısmi arazi kontrolü yapılıp firmaya teslim edilecek(22.12.2025)
+02.01.2026 Firmaya 05.01.2026 teslim edilecek
+15.01.2026 Kroki kontrolünde
+31.01.2026 Kroki müh. kontrolünde
+11.02.2026 Askı imzalanıyor cuma asılacak</v>
       </c>
     </row>
     <row r="115" xml:space="preserve">
@@ -4948,13 +4949,14 @@
         <v>FİRMAYA TESLİM EDİLDİ</v>
       </c>
       <c r="M116" t="str" xml:space="preserve">
-        <v xml:space="preserve">01.11.2025 firmaya teslim edilecek_x000d_
-05.11.2025 kontroller devam ediyor_x000d_
-13.11.2025 Firmaya 28.11.2025 teslim edilecek_x000d_
-02.12.2025 Firmaya 05.12.2025 teslim edilecek_x000d_
-15.12.2025 Değerlendirme devam ediyor_x000d_
-02.01.2026 Firmaya 15.01.2026 Teslim edilecek_x000d_
-31.01.2026 firma projeyi hazırlıyor 16.02.2026 tamamlayacak</v>
+        <v xml:space="preserve">01.11.2025 firmaya teslim edilecek
+05.11.2025 kontroller devam ediyor
+13.11.2025 Firmaya 28.11.2025 teslim edilecek
+02.12.2025 Firmaya 05.12.2025 teslim edilecek
+15.12.2025 Değerlendirme devam ediyor
+02.01.2026 Firmaya 15.01.2026 Teslim edilecek
+31.01.2026 firma projeyi hazırlıyor 16.02.2026 tamamlayacak
+11.02.2026 krokileri firma hazırlıyor</v>
       </c>
     </row>
     <row r="117" xml:space="preserve">
@@ -5045,17 +5047,18 @@
         <v>FİRMAYA TESLİM EDİLDİ</v>
       </c>
       <c r="M118" t="str" xml:space="preserve">
-        <v xml:space="preserve">01.11.2025 firmaya teslim edilecek_x000d_
-05.11.2025 kontroller devam ediyor_x000d_
-31.01.2026 firma kroki hazırlıyor_x000d_
-10.11.2025 Değerlendrime 13.11.2025 de bitecek_x000d_
-13.11.2025 Firmaya 17-21 haftası teslim edilecek_x000d_
-20.11.2025 firmaya 24.11.2025 de teslim edilecek_x000d_
-02.12.2025 bugün firmaya teslim edilecek_x000d_
-15.12.2025 Proje hazırlanıyor_x000d_
-22.12.2025 Proje 25.12.2025 biticek, krokiler 30.12.2025 verilecek_x000d_
-02.01.2026 Firma projeyi hazırlıyor _x000d_
-15.01.2026 kroki hazırlanıyor</v>
+        <v xml:space="preserve">01.11.2025 firmaya teslim edilecek
+05.11.2025 kontroller devam ediyor
+31.01.2026 firma kroki hazırlıyor
+10.11.2025 Değerlendrime 13.11.2025 de bitecek
+13.11.2025 Firmaya 17-21 haftası teslim edilecek
+20.11.2025 firmaya 24.11.2025 de teslim edilecek
+02.12.2025 bugün firmaya teslim edilecek
+15.12.2025 Proje hazırlanıyor
+22.12.2025 Proje 25.12.2025 biticek, krokiler 30.12.2025 verilecek
+02.01.2026 Firma projeyi hazırlıyor 
+15.01.2026 kroki hazırlanıyor
+11.02.2026 Kroki kontrolü yapılıyor. Tutanak basılacak 16-20.02 askı</v>
       </c>
     </row>
     <row r="119" xml:space="preserve">

</xml_diff>

<commit_message>
İş Takip Güncellemesi - 12.02.2026 09:33:56
</commit_message>
<xml_diff>
--- a/istakip.xlsx
+++ b/istakip.xlsx
@@ -7784,7 +7784,7 @@
         <v/>
       </c>
       <c r="L189" t="str">
-        <v>ÇALIŞMA PROGRAMINA ALINDI</v>
+        <v>KESİN ASKIDA</v>
       </c>
     </row>
     <row r="190">
@@ -7822,7 +7822,7 @@
         <v/>
       </c>
       <c r="L190" t="str">
-        <v>ÇALIŞMA PROGRAMINA ALINDI</v>
+        <v>KESİN ASKIDA</v>
       </c>
     </row>
     <row r="191">
@@ -7860,7 +7860,7 @@
         <v/>
       </c>
       <c r="L191" t="str">
-        <v>ÇALIŞMA PROGRAMINA ALINDI</v>
+        <v>KESİN ASKIDA</v>
       </c>
     </row>
     <row r="192">

</xml_diff>

<commit_message>
İş Takip Güncellemesi - 16.02.2026 10:32:24
</commit_message>
<xml_diff>
--- a/istakip.xlsx
+++ b/istakip.xlsx
@@ -4851,7 +4851,7 @@
         <v>2025-05-23</v>
       </c>
       <c r="L114" t="str">
-        <v>ASKI İLANINA HAZIRLANIYOR</v>
+        <v>BİLGİLENDİRME İLANINDA</v>
       </c>
       <c r="M114" t="str" xml:space="preserve">
         <v xml:space="preserve">14.11.2025 firmaya teslim edilecek
@@ -9477,13 +9477,13 @@
         <v>Yapıldı</v>
       </c>
       <c r="K21" t="str">
-        <v>Firmaya Teslim Edildi</v>
+        <v>Yapıldı</v>
       </c>
       <c r="L21" t="str">
         <v/>
       </c>
       <c r="M21" t="str">
-        <v/>
+        <v>2026-02-17</v>
       </c>
       <c r="N21" t="str">
         <v/>

</xml_diff>

<commit_message>
İş Takip Güncellemesi - 17.02.2026 15:28:16
</commit_message>
<xml_diff>
--- a/istakip.xlsx
+++ b/istakip.xlsx
@@ -2655,7 +2655,7 @@
         <v>2025-10-31</v>
       </c>
       <c r="L59" t="str">
-        <v>KESİN ASKIDA</v>
+        <v>DEVİR YAPILDI</v>
       </c>
     </row>
     <row r="60">
@@ -3117,7 +3117,7 @@
         <v>2025-10-31</v>
       </c>
       <c r="L71" t="str">
-        <v>KESİN ASKIDA</v>
+        <v>DEVİR YAPILDI</v>
       </c>
     </row>
     <row r="72">
@@ -3193,7 +3193,7 @@
         <v>2025-10-31</v>
       </c>
       <c r="L73" t="str">
-        <v>KESİN ASKIDA</v>
+        <v>DEVİR YAPILDI</v>
       </c>
     </row>
     <row r="74">
@@ -3231,7 +3231,7 @@
         <v>2025-10-31</v>
       </c>
       <c r="L74" t="str">
-        <v>KESİN ASKIDA</v>
+        <v>DEVİR YAPILDI</v>
       </c>
     </row>
     <row r="75">
@@ -3269,7 +3269,7 @@
         <v>2025-10-31</v>
       </c>
       <c r="L75" t="str">
-        <v>KESİN ASKIDA</v>
+        <v>DEVİR YAPILDI</v>
       </c>
     </row>
     <row r="76">
@@ -3842,7 +3842,7 @@
         <v>2025-10-31</v>
       </c>
       <c r="L90" t="str">
-        <v>KESİN ASKIDA</v>
+        <v>DEVİR YAPILDI</v>
       </c>
     </row>
     <row r="91">
@@ -3918,7 +3918,7 @@
         <v>2025-10-31</v>
       </c>
       <c r="L92" t="str">
-        <v>KESİN ASKIDA</v>
+        <v>DEVİR YAPILDI</v>
       </c>
     </row>
     <row r="93">
@@ -3956,7 +3956,7 @@
         <v>2025-10-31</v>
       </c>
       <c r="L93" t="str">
-        <v>KESİN ASKIDA</v>
+        <v>DEVİR YAPILDI</v>
       </c>
     </row>
     <row r="94">

</xml_diff>

<commit_message>
İş Takip Güncellemesi - 17.02.2026 15:32:19
</commit_message>
<xml_diff>
--- a/istakip.xlsx
+++ b/istakip.xlsx
@@ -3307,7 +3307,7 @@
         <v>2025-10-31</v>
       </c>
       <c r="L76" t="str">
-        <v>KESİN ASKIDA</v>
+        <v>DEVİR YAPILDI</v>
       </c>
     </row>
     <row r="77">
@@ -3383,7 +3383,7 @@
         <v>2025-10-31</v>
       </c>
       <c r="L78" t="str">
-        <v>KESİN ASKIDA</v>
+        <v>DEVİR YAPILDI</v>
       </c>
     </row>
     <row r="79">
@@ -3421,7 +3421,7 @@
         <v>2025-10-31</v>
       </c>
       <c r="L79" t="str">
-        <v>KESİN ASKIDA</v>
+        <v>DEVİR YAPILDI</v>
       </c>
     </row>
     <row r="80">
@@ -3459,7 +3459,7 @@
         <v>2025-10-31</v>
       </c>
       <c r="L80" t="str">
-        <v>KESİN ASKIDA</v>
+        <v>DEVİR YAPILDI</v>
       </c>
     </row>
     <row r="81">
@@ -3538,7 +3538,7 @@
         <v>2025-10-31</v>
       </c>
       <c r="L82" t="str">
-        <v>KESİN ASKIDA</v>
+        <v>DEVİR YAPILDI</v>
       </c>
     </row>
     <row r="83">
@@ -3576,7 +3576,7 @@
         <v>2025-10-31</v>
       </c>
       <c r="L83" t="str">
-        <v>KESİN ASKIDA</v>
+        <v>DEVİR YAPILDI</v>
       </c>
     </row>
     <row r="84">

</xml_diff>

<commit_message>
İş Takip Güncellemesi - 18.02.2026 11:06:42
</commit_message>
<xml_diff>
--- a/istakip.xlsx
+++ b/istakip.xlsx
@@ -4898,7 +4898,7 @@
         <v>2025-05-23</v>
       </c>
       <c r="L115" t="str">
-        <v>FİRMAYA TESLİM EDİLDİ</v>
+        <v>KROKİ/TUTANAK KONTROLÜ</v>
       </c>
       <c r="M115" t="str" xml:space="preserve">
         <v xml:space="preserve">Kıymetlendirmede eksiklikler var firma tamamlayacak bu hafta(20.10.2025)_x000d_
@@ -4946,7 +4946,7 @@
         <v>2025-05-23</v>
       </c>
       <c r="L116" t="str">
-        <v>FİRMAYA TESLİM EDİLDİ</v>
+        <v>KROKİ/TUTANAK KONTROLÜ</v>
       </c>
       <c r="M116" t="str" xml:space="preserve">
         <v xml:space="preserve">01.11.2025 firmaya teslim edilecek
@@ -4994,7 +4994,7 @@
         <v>2025-05-23</v>
       </c>
       <c r="L117" t="str">
-        <v>KROKİ/TUTANAK KONTROLÜ</v>
+        <v>ASKI İLANINA HAZIRLANIYOR</v>
       </c>
       <c r="M117" t="str" xml:space="preserve">
         <v xml:space="preserve">01.11.2025 firmaya teslim edilecek_x000d_
@@ -5044,7 +5044,7 @@
         <v>2025-05-23</v>
       </c>
       <c r="L118" t="str">
-        <v>FİRMAYA TESLİM EDİLDİ</v>
+        <v>KROKİ/TUTANAK KONTROLÜ</v>
       </c>
       <c r="M118" t="str" xml:space="preserve">
         <v xml:space="preserve">01.11.2025 firmaya teslim edilecek

</xml_diff>

<commit_message>
İş Takip Güncellemesi - 18.02.2026 12:26:20
</commit_message>
<xml_diff>
--- a/istakip.xlsx
+++ b/istakip.xlsx
@@ -1705,7 +1705,7 @@
         <v>2025-10-31</v>
       </c>
       <c r="L34" t="str">
-        <v>KESİN ASKIDA</v>
+        <v>DEVİR YAPILDI</v>
       </c>
     </row>
     <row r="35">
@@ -1781,7 +1781,7 @@
         <v>2025-10-31</v>
       </c>
       <c r="L36" t="str">
-        <v>KESİN ASKIDA</v>
+        <v>DEVİR YAPILDI</v>
       </c>
     </row>
     <row r="37">
@@ -1819,7 +1819,7 @@
         <v>2025-10-31</v>
       </c>
       <c r="L37" t="str">
-        <v>KESİN ASKIDA</v>
+        <v>DEVİR YAPILDI</v>
       </c>
     </row>
     <row r="38">
@@ -1857,7 +1857,7 @@
         <v>2025-10-31</v>
       </c>
       <c r="L38" t="str">
-        <v>KESİN ASKIDA</v>
+        <v>DEVİR YAPILDI</v>
       </c>
     </row>
     <row r="39">
@@ -1895,7 +1895,7 @@
         <v>2025-10-31</v>
       </c>
       <c r="L39" t="str">
-        <v>KESİN ASKIDA</v>
+        <v>DEVİR YAPILDI</v>
       </c>
     </row>
     <row r="40">
@@ -2009,7 +2009,7 @@
         <v>2025-10-31</v>
       </c>
       <c r="L42" t="str">
-        <v>KESİN ASKIDA</v>
+        <v>DEVİR YAPILDI</v>
       </c>
     </row>
     <row r="43">
@@ -2085,7 +2085,7 @@
         <v>2025-10-31</v>
       </c>
       <c r="L44" t="str">
-        <v>KESİN ASKIDA</v>
+        <v>DEVİR YAPILDI</v>
       </c>
     </row>
     <row r="45">
@@ -2123,7 +2123,7 @@
         <v>2025-10-31</v>
       </c>
       <c r="L45" t="str">
-        <v>KESİN ASKIDA</v>
+        <v>DEVİR YAPILDI</v>
       </c>
     </row>
     <row r="46">
@@ -2161,7 +2161,7 @@
         <v>2025-10-31</v>
       </c>
       <c r="L46" t="str">
-        <v>KESİN ASKIDA</v>
+        <v>DEVİR YAPILDI</v>
       </c>
     </row>
     <row r="47">
@@ -2199,7 +2199,7 @@
         <v>2025-10-31</v>
       </c>
       <c r="L47" t="str">
-        <v>KESİN ASKIDA</v>
+        <v>DEVİR YAPILDI</v>
       </c>
     </row>
     <row r="48">

</xml_diff>

<commit_message>
İş Takip Güncellemesi - 18.02.2026 12:45:02
</commit_message>
<xml_diff>
--- a/istakip.xlsx
+++ b/istakip.xlsx
@@ -863,7 +863,7 @@
         <v/>
       </c>
       <c r="L12" t="str">
-        <v>KROKİ/TUTANAK KONTROLÜ</v>
+        <v>ASKI İLANINA HAZIRLANIYOR</v>
       </c>
     </row>
     <row r="13">
@@ -1325,7 +1325,7 @@
         <v/>
       </c>
       <c r="L24" t="str">
-        <v>ÇALIŞMA ALANI İLANI YAPILDI</v>
+        <v>ARAZİ DEVAM EDİYOR</v>
       </c>
     </row>
     <row r="25">
@@ -1401,7 +1401,7 @@
         <v/>
       </c>
       <c r="L26" t="str">
-        <v>KROKİ/TUTANAK KONTROLÜ</v>
+        <v>ASKI İLANINA HAZIRLANIYOR</v>
       </c>
     </row>
     <row r="27">
@@ -1477,7 +1477,7 @@
         <v/>
       </c>
       <c r="L28" t="str">
-        <v>KROKİ/TUTANAK KONTROLÜ</v>
+        <v>ASKI İLANINA HAZIRLANIYOR</v>
       </c>
     </row>
     <row r="29">

</xml_diff>

<commit_message>
İş Takip Güncellemesi - 18.02.2026 13:21:08
</commit_message>
<xml_diff>
--- a/istakip.xlsx
+++ b/istakip.xlsx
@@ -597,7 +597,7 @@
         <v>2025-10-29</v>
       </c>
       <c r="L5" t="str">
-        <v>KESİN ASKIDA</v>
+        <v>DEVİR YAPILDI</v>
       </c>
     </row>
     <row r="6">
@@ -635,7 +635,7 @@
         <v>2025-10-29</v>
       </c>
       <c r="L6" t="str">
-        <v>KESİN ASKIDA</v>
+        <v>DEVİR YAPILDI</v>
       </c>
     </row>
     <row r="7">
@@ -711,7 +711,7 @@
         <v>2025-10-29</v>
       </c>
       <c r="L8" t="str">
-        <v>KESİN ASKIDA</v>
+        <v>DEVİR YAPILDI</v>
       </c>
     </row>
     <row r="9">
@@ -749,7 +749,7 @@
         <v>2025-10-29</v>
       </c>
       <c r="L9" t="str">
-        <v>KESİN ASKIDA</v>
+        <v>DEVİR YAPILDI</v>
       </c>
     </row>
     <row r="10">
@@ -787,7 +787,7 @@
         <v>2025-10-29</v>
       </c>
       <c r="L10" t="str">
-        <v>KESİN ASKIDA</v>
+        <v>DEVİR YAPILDI</v>
       </c>
     </row>
     <row r="11">

</xml_diff>

<commit_message>
İş Takip Güncellemesi - 18.02.2026 13:45:53
</commit_message>
<xml_diff>
--- a/istakip.xlsx
+++ b/istakip.xlsx
@@ -1971,7 +1971,7 @@
         <v>2025-10-31</v>
       </c>
       <c r="L41" t="str">
-        <v>KESİN ASKIDA</v>
+        <v>DEVİR YAPILDI</v>
       </c>
     </row>
     <row r="42">
@@ -2047,7 +2047,7 @@
         <v>2025-10-31</v>
       </c>
       <c r="L43" t="str">
-        <v>KESİN ASKIDA</v>
+        <v>DEVİR YAPILDI</v>
       </c>
     </row>
     <row r="44">

</xml_diff>

<commit_message>
İş Takip Güncellemesi - 18.02.2026 17:16:03
</commit_message>
<xml_diff>
--- a/istakip.xlsx
+++ b/istakip.xlsx
@@ -3690,7 +3690,7 @@
         <v>2025-10-31</v>
       </c>
       <c r="L86" t="str">
-        <v>KESİN ASKIDA</v>
+        <v>DEVİR YAPILDI</v>
       </c>
     </row>
     <row r="87">
@@ -3728,7 +3728,7 @@
         <v>2025-10-31</v>
       </c>
       <c r="L87" t="str">
-        <v>KESİN ASKIDA</v>
+        <v>DEVİR YAPILDI</v>
       </c>
     </row>
     <row r="88">
@@ -3766,7 +3766,7 @@
         <v>2025-10-31</v>
       </c>
       <c r="L88" t="str">
-        <v>KESİN ASKIDA</v>
+        <v>DEVİR YAPILDI</v>
       </c>
     </row>
     <row r="89">

</xml_diff>

<commit_message>
İş Takip Güncellemesi - 18.02.2026 17:17:04
</commit_message>
<xml_diff>
--- a/istakip.xlsx
+++ b/istakip.xlsx
@@ -3614,7 +3614,7 @@
         <v>2025-10-31</v>
       </c>
       <c r="L84" t="str">
-        <v>KESİN ASKIDA</v>
+        <v>DEVİR YAPILDI</v>
       </c>
     </row>
     <row r="85">
@@ -3804,7 +3804,7 @@
         <v>2025-10-31</v>
       </c>
       <c r="L89" t="str">
-        <v>KESİN ASKIDA</v>
+        <v>DEVİR YAPILDI</v>
       </c>
     </row>
     <row r="90">

</xml_diff>

<commit_message>
İş Takip Güncellemesi - 19.02.2026 11:08:23
</commit_message>
<xml_diff>
--- a/istakip.xlsx
+++ b/istakip.xlsx
@@ -2693,7 +2693,7 @@
         <v>2025-10-31</v>
       </c>
       <c r="L60" t="str">
-        <v>KESİN ASKIDA</v>
+        <v>DEVİR YAPILDI</v>
       </c>
     </row>
     <row r="61">
@@ -2769,7 +2769,7 @@
         <v>2025-10-31</v>
       </c>
       <c r="L62" t="str">
-        <v>KESİN ASKIDA</v>
+        <v>DEVİR YAPILDI</v>
       </c>
     </row>
     <row r="63">

</xml_diff>

<commit_message>
İş Takip Güncellemesi - 20.02.2026 14:36:20
</commit_message>
<xml_diff>
--- a/istakip.xlsx
+++ b/istakip.xlsx
@@ -4032,7 +4032,7 @@
         <v>2025-05-23</v>
       </c>
       <c r="L95" t="str">
-        <v>KESİN ASKIDAN İNDİ. BEKLEMEDE</v>
+        <v>DEVİR YAPILDI</v>
       </c>
     </row>
     <row r="96">
@@ -4108,7 +4108,7 @@
         <v>2025-05-23</v>
       </c>
       <c r="L97" t="str">
-        <v>KESİN ASKIDAN İNDİ. BEKLEMEDE</v>
+        <v>DEVİR YAPILDI</v>
       </c>
     </row>
     <row r="98" xml:space="preserve">

</xml_diff>

<commit_message>
İş Takip Güncellemesi - 23.02.2026 14:36:51
</commit_message>
<xml_diff>
--- a/istakip.xlsx
+++ b/istakip.xlsx
@@ -9,6 +9,7 @@
     <sheet name="İlçe" sheetId="4" r:id="rId4"/>
     <sheet name="Uygulama" sheetId="5" r:id="rId5"/>
     <sheet name="Liste" sheetId="6" r:id="rId6"/>
+    <sheet name="Komisyon" sheetId="7" r:id="rId7"/>
   </sheets>
 </workbook>
 </file>
@@ -4994,7 +4995,7 @@
         <v>2025-05-23</v>
       </c>
       <c r="L117" t="str">
-        <v>ASKI İLANINA HAZIRLANIYOR</v>
+        <v>BİLGİLENDİRME İLANINDA</v>
       </c>
       <c r="M117" t="str" xml:space="preserve">
         <v xml:space="preserve">01.11.2025 firmaya teslim edilecek_x000d_
@@ -9618,13 +9619,13 @@
         <v>Yapıldı</v>
       </c>
       <c r="K24" t="str">
-        <v>Firmaya Teslim Edildi</v>
+        <v>Yapıldı</v>
       </c>
       <c r="L24" t="str">
         <v/>
       </c>
       <c r="M24" t="str">
-        <v/>
+        <v>2026-02-24</v>
       </c>
       <c r="N24" t="str">
         <v/>
@@ -13539,4 +13540,1019 @@
     <ignoredError numberStoredAsText="1" sqref="A1:D26"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C91"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>İLÇE</v>
+      </c>
+      <c r="B1" t="str">
+        <v>BİRİM</v>
+      </c>
+      <c r="C1" t="str">
+        <v>KOMİSYON GÖREVLİLERİ</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Akdeniz</v>
+      </c>
+      <c r="B2" t="str">
+        <v>AKDAM</v>
+      </c>
+      <c r="C2" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Akdeniz</v>
+      </c>
+      <c r="B3" t="str">
+        <v>ESENLİ</v>
+      </c>
+      <c r="C3" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Akdeniz</v>
+      </c>
+      <c r="B4" t="str">
+        <v>HEBİLLİ</v>
+      </c>
+      <c r="C4" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Toroslar</v>
+      </c>
+      <c r="B5" t="str">
+        <v>BEKİRALANI</v>
+      </c>
+      <c r="C5" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>Toroslar</v>
+      </c>
+      <c r="B6" t="str">
+        <v>ÇELEBİLİ</v>
+      </c>
+      <c r="C6" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>Toroslar</v>
+      </c>
+      <c r="B7" t="str">
+        <v>DARISEKİSİ</v>
+      </c>
+      <c r="C7" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>Toroslar</v>
+      </c>
+      <c r="B8" t="str">
+        <v>DÜĞDÜÖREN</v>
+      </c>
+      <c r="C8" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>Toroslar</v>
+      </c>
+      <c r="B9" t="str">
+        <v>EVCİLİ</v>
+      </c>
+      <c r="C9" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>Toroslar</v>
+      </c>
+      <c r="B10" t="str">
+        <v>KORUCULAR</v>
+      </c>
+      <c r="C10" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>Toroslar</v>
+      </c>
+      <c r="B11" t="str">
+        <v>MUSALI</v>
+      </c>
+      <c r="C11" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>Tarsus</v>
+      </c>
+      <c r="B12" t="str">
+        <v>GÖÇÜK</v>
+      </c>
+      <c r="C12" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>Tarsus</v>
+      </c>
+      <c r="B13" t="str">
+        <v>KIZILÇUKUR</v>
+      </c>
+      <c r="C13" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>Tarsus</v>
+      </c>
+      <c r="B14" t="str">
+        <v>KARAKÜTÜK</v>
+      </c>
+      <c r="C14" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>Tarsus</v>
+      </c>
+      <c r="B15" t="str">
+        <v>ESKİŞEHİR</v>
+      </c>
+      <c r="C15" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>Tarsus</v>
+      </c>
+      <c r="B16" t="str">
+        <v>KERİMLER</v>
+      </c>
+      <c r="C16" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>Tarsus</v>
+      </c>
+      <c r="B17" t="str">
+        <v>TAŞÇILI</v>
+      </c>
+      <c r="C17" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>Tarsus</v>
+      </c>
+      <c r="B18" t="str">
+        <v>İNCİRGEDİĞİ</v>
+      </c>
+      <c r="C18" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>Tarsus</v>
+      </c>
+      <c r="B19" t="str">
+        <v>KADELLİ</v>
+      </c>
+      <c r="C19" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>Tarsus</v>
+      </c>
+      <c r="B20" t="str">
+        <v>CİNKÖY</v>
+      </c>
+      <c r="C20" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>Tarsus</v>
+      </c>
+      <c r="B21" t="str">
+        <v>İNKÖY</v>
+      </c>
+      <c r="C21" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>Tarsus</v>
+      </c>
+      <c r="B22" t="str">
+        <v>OLUKKOYAĞI</v>
+      </c>
+      <c r="C22" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>Mezitli</v>
+      </c>
+      <c r="B23" t="str">
+        <v>BOZÖN</v>
+      </c>
+      <c r="C23" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>Toroslar</v>
+      </c>
+      <c r="B24" t="str">
+        <v>BELENKEŞLİK</v>
+      </c>
+      <c r="C24" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>Toroslar</v>
+      </c>
+      <c r="B25" t="str">
+        <v>DORUKLU</v>
+      </c>
+      <c r="C25" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>Toroslar</v>
+      </c>
+      <c r="B26" t="str">
+        <v>GÖZNE</v>
+      </c>
+      <c r="C26" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>Toroslar</v>
+      </c>
+      <c r="B27" t="str">
+        <v>KAŞLI</v>
+      </c>
+      <c r="C27" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>Toroslar</v>
+      </c>
+      <c r="B28" t="str">
+        <v>RESULKÖY</v>
+      </c>
+      <c r="C28" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>Yenişehir</v>
+      </c>
+      <c r="B29" t="str">
+        <v>EMİRLER</v>
+      </c>
+      <c r="C29" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>Anamur</v>
+      </c>
+      <c r="B30" t="str">
+        <v>AŞAĞIKÜKÜR</v>
+      </c>
+      <c r="C30" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>Anamur</v>
+      </c>
+      <c r="B31" t="str">
+        <v>BOZDOĞAN</v>
+      </c>
+      <c r="C31" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>Anamur</v>
+      </c>
+      <c r="B32" t="str">
+        <v>BOĞUNTU</v>
+      </c>
+      <c r="C32" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>Anamur</v>
+      </c>
+      <c r="B33" t="str">
+        <v>ÇAMLIPINAR</v>
+      </c>
+      <c r="C33" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>Anamur</v>
+      </c>
+      <c r="B34" t="str">
+        <v>ÇAMLIPINARALANI</v>
+      </c>
+      <c r="C34" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>Anamur</v>
+      </c>
+      <c r="B35" t="str">
+        <v>ÇATALOLUK</v>
+      </c>
+      <c r="C35" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>Anamur</v>
+      </c>
+      <c r="B36" t="str">
+        <v>ÇUKURABANOZ</v>
+      </c>
+      <c r="C36" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>Anamur</v>
+      </c>
+      <c r="B37" t="str">
+        <v>DEMİRÖREN</v>
+      </c>
+      <c r="C37" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>Anamur</v>
+      </c>
+      <c r="B38" t="str">
+        <v>GÜNGÖREN</v>
+      </c>
+      <c r="C38" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>Anamur</v>
+      </c>
+      <c r="B39" t="str">
+        <v>KALINÖREN</v>
+      </c>
+      <c r="C39" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>Anamur</v>
+      </c>
+      <c r="B40" t="str">
+        <v>KARAÇUKUR</v>
+      </c>
+      <c r="C40" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>Anamur</v>
+      </c>
+      <c r="B41" t="str">
+        <v>KARALARBAHŞİŞ</v>
+      </c>
+      <c r="C41" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>Anamur</v>
+      </c>
+      <c r="B42" t="str">
+        <v>KARAAĞA</v>
+      </c>
+      <c r="C42" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>Anamur</v>
+      </c>
+      <c r="B43" t="str">
+        <v>KORUCUK</v>
+      </c>
+      <c r="C43" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>Anamur</v>
+      </c>
+      <c r="B44" t="str">
+        <v>MALAKLAR</v>
+      </c>
+      <c r="C44" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>Anamur</v>
+      </c>
+      <c r="B45" t="str">
+        <v>NASRADDİN</v>
+      </c>
+      <c r="C45" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>Anamur</v>
+      </c>
+      <c r="B46" t="str">
+        <v>ORMANCIK</v>
+      </c>
+      <c r="C46" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>Anamur</v>
+      </c>
+      <c r="B47" t="str">
+        <v>ORTAKÖY</v>
+      </c>
+      <c r="C47" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>Anamur</v>
+      </c>
+      <c r="B48" t="str">
+        <v>SUGÖZÜ</v>
+      </c>
+      <c r="C48" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>Anamur</v>
+      </c>
+      <c r="B49" t="str">
+        <v>SARIAĞAÇ</v>
+      </c>
+      <c r="C49" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v>Anamur</v>
+      </c>
+      <c r="B50" t="str">
+        <v>SARIDANA</v>
+      </c>
+      <c r="C50" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v>Anamur</v>
+      </c>
+      <c r="B51" t="str">
+        <v>YUKARIKÜKÜR</v>
+      </c>
+      <c r="C51" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="str">
+        <v>Aydıncık</v>
+      </c>
+      <c r="B52" t="str">
+        <v>HACIBAHATTİN</v>
+      </c>
+      <c r="C52" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="str">
+        <v>Bozyazı</v>
+      </c>
+      <c r="B53" t="str">
+        <v>BAHÇEKOYAĞI</v>
+      </c>
+      <c r="C53" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="str">
+        <v>Bozyazı</v>
+      </c>
+      <c r="B54" t="str">
+        <v>BEYRELİ</v>
+      </c>
+      <c r="C54" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="str">
+        <v>Bozyazı</v>
+      </c>
+      <c r="B55" t="str">
+        <v>ELMAKUZU</v>
+      </c>
+      <c r="C55" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="str">
+        <v>Bozyazı</v>
+      </c>
+      <c r="B56" t="str">
+        <v>GÖZCE</v>
+      </c>
+      <c r="C56" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="str">
+        <v>Bozyazı</v>
+      </c>
+      <c r="B57" t="str">
+        <v>GÖZSÜZCE</v>
+      </c>
+      <c r="C57" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="str">
+        <v>Bozyazı</v>
+      </c>
+      <c r="B58" t="str">
+        <v>KÖMÜRLÜ</v>
+      </c>
+      <c r="C58" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="str">
+        <v>Bozyazı</v>
+      </c>
+      <c r="B59" t="str">
+        <v>LENGER</v>
+      </c>
+      <c r="C59" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="str">
+        <v>Bozyazı</v>
+      </c>
+      <c r="B60" t="str">
+        <v>KIZILCA</v>
+      </c>
+      <c r="C60" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="str">
+        <v>Bozyazı</v>
+      </c>
+      <c r="B61" t="str">
+        <v>TEKEDÜZÜ</v>
+      </c>
+      <c r="C61" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="str">
+        <v>Bozyazı</v>
+      </c>
+      <c r="B62" t="str">
+        <v>DEREKÖY</v>
+      </c>
+      <c r="C62" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="str">
+        <v>Gülnar</v>
+      </c>
+      <c r="B63" t="str">
+        <v>BÜYÜKECELİ</v>
+      </c>
+      <c r="C63" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="str">
+        <v>Gülnar</v>
+      </c>
+      <c r="B64" t="str">
+        <v>ŞEYHÖMER</v>
+      </c>
+      <c r="C64" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="str">
+        <v>Gülnar</v>
+      </c>
+      <c r="B65" t="str">
+        <v>ZEYNE(SÜTLÜCE)</v>
+      </c>
+      <c r="C65" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="str">
+        <v>Silifke</v>
+      </c>
+      <c r="B66" t="str">
+        <v>ALTINKUM</v>
+      </c>
+      <c r="C66" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="str">
+        <v>Silifke</v>
+      </c>
+      <c r="B67" t="str">
+        <v>ARKARASI</v>
+      </c>
+      <c r="C67" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="str">
+        <v>Silifke</v>
+      </c>
+      <c r="B68" t="str">
+        <v>ATİK</v>
+      </c>
+      <c r="C68" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="str">
+        <v>Silifke</v>
+      </c>
+      <c r="B69" t="str">
+        <v>BOYNUİNCELİ</v>
+      </c>
+      <c r="C69" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="str">
+        <v>Silifke</v>
+      </c>
+      <c r="B70" t="str">
+        <v>BURUNUCU</v>
+      </c>
+      <c r="C70" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="str">
+        <v>Silifke</v>
+      </c>
+      <c r="B71" t="str">
+        <v>ÇELTİKÇİ</v>
+      </c>
+      <c r="C71" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="str">
+        <v>Silifke</v>
+      </c>
+      <c r="B72" t="str">
+        <v>GÜLÜMPAŞALI</v>
+      </c>
+      <c r="C72" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="str">
+        <v>Silifke</v>
+      </c>
+      <c r="B73" t="str">
+        <v>HIRMANLI</v>
+      </c>
+      <c r="C73" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="str">
+        <v>Silifke</v>
+      </c>
+      <c r="B74" t="str">
+        <v>CILBAYIR</v>
+      </c>
+      <c r="C74" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="str">
+        <v>Silifke</v>
+      </c>
+      <c r="B75" t="str">
+        <v>İMAMUŞAĞI</v>
+      </c>
+      <c r="C75" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="str">
+        <v>Silifke</v>
+      </c>
+      <c r="B76" t="str">
+        <v>KAVAK</v>
+      </c>
+      <c r="C76" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="str">
+        <v>Silifke</v>
+      </c>
+      <c r="B77" t="str">
+        <v>KURTULUŞ</v>
+      </c>
+      <c r="C77" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="str">
+        <v>Silifke</v>
+      </c>
+      <c r="B78" t="str">
+        <v>MARA</v>
+      </c>
+      <c r="C78" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="str">
+        <v>Silifke</v>
+      </c>
+      <c r="B79" t="str">
+        <v>NASRULLAH</v>
+      </c>
+      <c r="C79" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="str">
+        <v>Silifke</v>
+      </c>
+      <c r="B80" t="str">
+        <v>SEYDİLİ</v>
+      </c>
+      <c r="C80" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="str">
+        <v>Silifke</v>
+      </c>
+      <c r="B81" t="str">
+        <v>SÖKÜN</v>
+      </c>
+      <c r="C81" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="str">
+        <v>Silifke</v>
+      </c>
+      <c r="B82" t="str">
+        <v>ULUGÖZ</v>
+      </c>
+      <c r="C82" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="str">
+        <v>Silifke</v>
+      </c>
+      <c r="B83" t="str">
+        <v>YEĞENLİ</v>
+      </c>
+      <c r="C83" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="str">
+        <v>Yenişehir</v>
+      </c>
+      <c r="B84" t="str">
+        <v>Turunçlu</v>
+      </c>
+      <c r="C84" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="str">
+        <v>Erdemli</v>
+      </c>
+      <c r="B85" t="str">
+        <v>Pınarbaşı</v>
+      </c>
+      <c r="C85" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="str">
+        <v>Toroslar</v>
+      </c>
+      <c r="B86" t="str">
+        <v>Tırtar</v>
+      </c>
+      <c r="C86" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="str">
+        <v>Toroslar</v>
+      </c>
+      <c r="B87" t="str">
+        <v>Arslanköy</v>
+      </c>
+      <c r="C87" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="str">
+        <v>Mut</v>
+      </c>
+      <c r="B88" t="str">
+        <v>Hacınuhlu</v>
+      </c>
+      <c r="C88" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="str">
+        <v>Silifke</v>
+      </c>
+      <c r="B89" t="str">
+        <v>Kızılisalı</v>
+      </c>
+      <c r="C89" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="str">
+        <v>Anamur</v>
+      </c>
+      <c r="B90" t="str">
+        <v>Lale</v>
+      </c>
+      <c r="C90" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="str">
+        <v>Bozyazı</v>
+      </c>
+      <c r="B91" t="str">
+        <v>Derebaşı</v>
+      </c>
+      <c r="C91" t="str">
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:C91"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
İş Takip Güncellemesi - 23.02.2026 14:45:58
</commit_message>
<xml_diff>
--- a/istakip.xlsx
+++ b/istakip.xlsx
@@ -5097,7 +5097,7 @@
         <v>2025-05-23</v>
       </c>
       <c r="L119" t="str">
-        <v>DEĞERLENDİRMEDE</v>
+        <v>FİRMAYA TESLİM EDİLDİ</v>
       </c>
       <c r="M119" t="str" xml:space="preserve">
         <v xml:space="preserve">15.12.2025 Değerlendirme devam ediyor_x000d_
@@ -5140,7 +5140,7 @@
         <v>2025-05-23</v>
       </c>
       <c r="L120" t="str">
-        <v>DEĞERLENDİRMEDE</v>
+        <v>İHALEDEN/PROGRAMDAN ÇIKARILDI</v>
       </c>
       <c r="M120" t="str" xml:space="preserve">
         <v xml:space="preserve">14.11.2025 firmaya teslim edilecek_x000d__x000d__x000d__x000d__x000d__x000d_

</xml_diff>

<commit_message>
İş Takip Güncellemesi - 24.02.2026 12:13:12
</commit_message>
<xml_diff>
--- a/istakip.xlsx
+++ b/istakip.xlsx
@@ -864,7 +864,7 @@
         <v/>
       </c>
       <c r="L12" t="str">
-        <v>ASKI İLANINA HAZIRLANIYOR</v>
+        <v>KESİN ASKIDA</v>
       </c>
     </row>
     <row r="13">
@@ -1402,7 +1402,7 @@
         <v/>
       </c>
       <c r="L26" t="str">
-        <v>ASKI İLANINA HAZIRLANIYOR</v>
+        <v>KESİN ASKIDA</v>
       </c>
     </row>
     <row r="27">
@@ -1478,7 +1478,7 @@
         <v/>
       </c>
       <c r="L28" t="str">
-        <v>ASKI İLANINA HAZIRLANIYOR</v>
+        <v>KESİN ASKIDA</v>
       </c>
     </row>
     <row r="29">

</xml_diff>

<commit_message>
İş Takip Güncellemesi - 26.02.2026 12:03:49
</commit_message>
<xml_diff>
--- a/istakip.xlsx
+++ b/istakip.xlsx
@@ -4150,9 +4150,10 @@
         <v>FİRMAYA TESLİM EDİLDİ</v>
       </c>
       <c r="M98" t="str" xml:space="preserve">
-        <v xml:space="preserve">Ormancı kontrolünde(13.10.2025)_x000d__x000d_
-GM OLUR'u beklenecek_x000d__x000d_
-31.01.2026 kroki basılıyor</v>
+        <v xml:space="preserve">Ormancı kontrolünde(13.10.2025)
+GM OLUR'u beklenecek
+31.01.2026 kroki basılıyor
+KROKİ/TUTANAK KONTROLLERİ TAMAMLANIP 02.03.2026 İLAN YAPILACAK</v>
       </c>
     </row>
     <row r="99">
@@ -4231,21 +4232,15 @@
         <v>BİLGİLENDİRME İLANINDA</v>
       </c>
       <c r="M100" t="str" xml:space="preserve">
-        <v xml:space="preserve">15.10.2025 Projesine başlanılacak(Ormancı kontrolünde)_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-01.11.2025 kroki basılacak_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-10.11.2025 Kroki kontrol için 11.11.2025 de verilecek. 14.11.2025 de firmaya teslim edilecek_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-02.12.025 tutanaklarına başlanılacak_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-16.12.2025 tutanaklarına başlanılacak_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-22.12.2025 tutanaklarına başlanılacak_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-06.01.2026 Askı yapılacak_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-19.01.2026 askı yapılacak</v>
+        <v xml:space="preserve">15.10.2025 Projesine başlanılacak(Ormancı kontrolünde)
+01.11.2025 kroki basılacak
+10.11.2025 Kroki kontrol için 11.11.2025 de verilecek. 14.11.2025 de firmaya teslim edilecek
+02.12.025 tutanaklarına başlanılacak
+16.12.2025 tutanaklarına başlanılacak
+22.12.2025 tutanaklarına başlanılacak
+06.01.2026 Askı yapılacak
+19.01.2026 askı yapılacak
+KOMİSYON TAMAMLANIP 25.02.2026 KESİN ASKIYA ÇIKACAK</v>
       </c>
     </row>
     <row r="101">
@@ -4327,18 +4322,19 @@
         <v>KROKİ/TUTANAK KONTROLÜ</v>
       </c>
       <c r="M102" t="str" xml:space="preserve">
-        <v xml:space="preserve">01.11.2025 firmaya teslim edilecek_x000d__x000d_
-07.11.2025 ormanı bakıp teslim edecek_x000d__x000d_
-10.11.2025 kontrol edilip firmaya teslim edilecek_x000d__x000d_
-10.11.2025 Ormancı 11.11.2025 teslim edecek_x000d__x000d_
-13.11.2025 Ormancı 17.11.2025 teslim edecek_x000d__x000d_
-20.11.2025 orman mükerrerliği ile ilgili beyanname düzenlendi tescili bekleniyor_x000d__x000d_
-02.12.2025 Krokilerine başlanıldı_x000d__x000d_
-15.12.2025 Proje hazırlanıyor_x000d__x000d_
-22.12.2025 Proje hazırlanıyor _x000d__x000d_
-05.01.2026 KROKİLERE BAŞLANACAK_x000d__x000d_
-15.01.2026 Devam ediyor firma_x000d__x000d_
-31.01.2026 Personel kontrolünde 09-13.02 askı ilanı yapılacak</v>
+        <v xml:space="preserve">01.11.2025 firmaya teslim edilecek
+07.11.2025 ormanı bakıp teslim edecek
+10.11.2025 kontrol edilip firmaya teslim edilecek
+10.11.2025 Ormancı 11.11.2025 teslim edecek
+13.11.2025 Ormancı 17.11.2025 teslim edecek
+20.11.2025 orman mükerrerliği ile ilgili beyanname düzenlendi tescili bekleniyor
+02.12.2025 Krokilerine başlanıldı
+15.12.2025 Proje hazırlanıyor
+22.12.2025 Proje hazırlanıyor 
+05.01.2026 KROKİLERE BAŞLANACAK
+15.01.2026 Devam ediyor firma
+31.01.2026 Personel kontrolünde 09-13.02 askı ilanı yapılacak
+26.02.2026 BİLGİLENDİRME İLANI YAPILACAK</v>
       </c>
     </row>
     <row r="103">
@@ -4496,16 +4492,17 @@
         <v>BİLGİLENDİRME İLANINDA</v>
       </c>
       <c r="M106" t="str" xml:space="preserve">
-        <v xml:space="preserve">03.11.2025 firmaya teslim edilecek_x000d__x000d_
-05.11.2025 kontroller devam ediyor 10.11.2025 bazı yerlerin arazi kontrolleri yapılacak_x000d__x000d_
-13.11.2025 arazi kontrolü 18.11.2025 de yapılıp, 21.11.2025 de firmaya teslim edilecek_x000d__x000d_
-20.11.2025 arazi kontrolü yapılıyor 24.11.2025 de firmaya teslim edilecek_x000d__x000d_
-02.12.2025 krokileri hazırlanıyor_x000d__x000d_
-15.12.2025 Krokileri basılıyor_x000d__x000d_
-22.12.2025 Kroki kontrolü 25.12.2025 biticek_x000d__x000d_
-02.01.2026 Tutanaklarına başlanıldı_x000d__x000d_
-15.01.2026 TEMUR beyin kontrolünde_x000d__x000d_
-31.01.2026 03.02 askı yapılacak</v>
+        <v xml:space="preserve">03.11.2025 firmaya teslim edilecek
+05.11.2025 kontroller devam ediyor 10.11.2025 bazı yerlerin arazi kontrolleri yapılacak
+13.11.2025 arazi kontrolü 18.11.2025 de yapılıp, 21.11.2025 de firmaya teslim edilecek
+20.11.2025 arazi kontrolü yapılıyor 24.11.2025 de firmaya teslim edilecek
+02.12.2025 krokileri hazırlanıyor
+15.12.2025 Krokileri basılıyor
+22.12.2025 Kroki kontrolü 25.12.2025 biticek
+02.01.2026 Tutanaklarına başlanıldı
+15.01.2026 TEMUR beyin kontrolünde
+31.01.2026 03.02 askı yapılacak
+BİLGİLENDİRME İLANINDA. KOMİSYON 26-27.02 YAPILIP KESİN ASKIYA 04.03 ÇIKILACAK</v>
       </c>
     </row>
     <row r="107" xml:space="preserve">
@@ -4546,12 +4543,13 @@
         <v>KESİN ASKIDA</v>
       </c>
       <c r="M107" t="str" xml:space="preserve">
-        <v xml:space="preserve">16.10.2025 firmaya teslim edilecek_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-26.10.2025 tutanak yazılacak_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-05.11.2025 kad. üyesinde tutanak notları düzenlemesi devam ettiğinden tutanaklara geçilemedi_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-10.11.2025 Tutanak 12.11.2025 de basılacak_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-13.11.2025 Tutanak imzaya 15-16.11.2025 de götürülecek_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-20.11.2025 24.11.2025 askıya çıkacak(tutanak kontrolü)</v>
+        <v xml:space="preserve">16.10.2025 firmaya teslim edilecek
+26.10.2025 tutanak yazılacak
+05.11.2025 kad. üyesinde tutanak notları düzenlemesi devam ettiğinden tutanaklara geçilemedi
+10.11.2025 Tutanak 12.11.2025 de basılacak
+13.11.2025 Tutanak imzaya 15-16.11.2025 de götürülecek
+20.11.2025 24.11.2025 askıya çıkacak(tutanak kontrolü)
+KOMİSYON TAMAMLANIP 23.02.2026 KESİN ASKIYA ÇIKACAK</v>
       </c>
     </row>
     <row r="108">
@@ -4671,13 +4669,14 @@
         <v>BİLGİLENDİRME İLANINDA</v>
       </c>
       <c r="M110" t="str" xml:space="preserve">
-        <v xml:space="preserve">16.10.2025 Taşçılı tutanak Kadastro Üyesine teslim edilecek._x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-28.10.2025 tutanak firmaya verilecek_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-30.10.2025 askıya çıkacak_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-30.10.2025 tutanak firmaya teslim edildi, hatalıların düzeltmesi devam ediyor_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-10.11.2025 Tutanak imzaya 12.11.2025 de götürülecek_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-13.11.2025 Askıya 18.11.2025 de çıkacak_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-20.11.2025 Askıya 24.11.2025 de çıkacak</v>
+        <v xml:space="preserve">16.10.2025 Taşçılı tutanak Kadastro Üyesine teslim edilecek.
+28.10.2025 tutanak firmaya verilecek
+30.10.2025 askıya çıkacak
+30.10.2025 tutanak firmaya teslim edildi, hatalıların düzeltmesi devam ediyor
+10.11.2025 Tutanak imzaya 12.11.2025 de götürülecek
+13.11.2025 Askıya 18.11.2025 de çıkacak
+20.11.2025 Askıya 24.11.2025 de çıkacak
+KOMİSYON TAMAMLANIP 25.02.2026 KESİN ASKIYA ÇIKACAK</v>
       </c>
     </row>
     <row r="111" xml:space="preserve">
@@ -4718,16 +4717,17 @@
         <v>BİLGİLENDİRME İLANINDA</v>
       </c>
       <c r="M111" t="str" xml:space="preserve">
-        <v xml:space="preserve">24.10.2025 firmaya teslim edilecek_x000d__x000d_
-28.10.2025 firmaya teslim edilecek_x000d__x000d_
-03.11.2025 ormancı kontrolünde_x000d__x000d_
-20.11.2025 ormancı kontrolünde_x000d__x000d_
-02.12.2025 Firmaya teslim edildi_x000d__x000d_
-15.12.2025 Proje hazırlanıyor_x000d__x000d_
-22.12.2025 Kroki hazırlanıyor. 26.12.205 de biticek_x000d__x000d_
-02.01.2026 Kroki kontrolüne 05.01.2026 başlanıp 08.01.2026 bitip tutanağa geçilecek _x000d__x000d_
-15.01.2026 Tutanak başlanılacak_x000d__x000d_
-31.01.2026 imza aşamasında haftaiçi askı yapılacak</v>
+        <v xml:space="preserve">24.10.2025 firmaya teslim edilecek
+28.10.2025 firmaya teslim edilecek
+03.11.2025 ormancı kontrolünde
+20.11.2025 ormancı kontrolünde
+02.12.2025 Firmaya teslim edildi
+15.12.2025 Proje hazırlanıyor
+22.12.2025 Kroki hazırlanıyor. 26.12.205 de biticek
+02.01.2026 Kroki kontrolüne 05.01.2026 başlanıp 08.01.2026 bitip tutanağa geçilecek 
+15.01.2026 Tutanak başlanılacak
+31.01.2026 imza aşamasında haftaiçi askı yapılacak
+BİLGİLENDİRME İLANINDA. KOMİSYON 03-04.03 YAPILIP KESİN ASKIYA 09.03 ÇIKILACAK</v>
       </c>
     </row>
     <row r="112">
@@ -4855,13 +4855,14 @@
         <v>BİLGİLENDİRME İLANINDA</v>
       </c>
       <c r="M114" t="str" xml:space="preserve">
-        <v xml:space="preserve">14.11.2025 firmaya teslim edilecek_x000d_
-02.12.2025 araziye çıkılacak_x000d_
-15.12.2025 Kısmi arazi kontrolü yapılıp firmaya teslim edilecek(22.12.2025)_x000d_
-02.01.2026 Firmaya 05.01.2026 teslim edilecek_x000d_
-15.01.2026 Kroki kontrolünde_x000d_
-31.01.2026 Kroki müh. kontrolünde_x000d_
-11.02.2026 Askı imzalanıyor cuma asılacak</v>
+        <v xml:space="preserve">14.11.2025 firmaya teslim edilecek
+02.12.2025 araziye çıkılacak
+15.12.2025 Kısmi arazi kontrolü yapılıp firmaya teslim edilecek(22.12.2025)
+02.01.2026 Firmaya 05.01.2026 teslim edilecek
+15.01.2026 Kroki kontrolünde
+31.01.2026 Kroki müh. kontrolünde
+11.02.2026 Askı imzalanıyor cuma asılacak
+BİLGİLENDİRME İLANINDA. KOMİSYON 05-06.03 YAPILIP KESİN ASKIYA 11.03 ÇIKILACAK</v>
       </c>
     </row>
     <row r="115" xml:space="preserve">
@@ -4902,14 +4903,15 @@
         <v>KROKİ/TUTANAK KONTROLÜ</v>
       </c>
       <c r="M115" t="str" xml:space="preserve">
-        <v xml:space="preserve">Kıymetlendirmede eksiklikler var firma tamamlayacak bu hafta(20.10.2025)_x000d__x000d_
-05.11.2025 eksik uçuşlar teslim edildi_x000d__x000d_
-10.11.2025 kıymetlendirmeler kontrol ediliyor_x000d__x000d_
-13.11.2025 Firmaya 28.11.2025 de teslim edilecek_x000d__x000d_
-15.12.2025 Değerlendirme devam ediyor_x000d__x000d_
-22.12.2025 Kısmi uçuş yapıldı kıymetlendirme yapılıyor aynı zamanda değerlendirme devam ediyor_x000d__x000d_
-02.01.2026 Değerlendirme 15.01.2026 biticek_x000d__x000d_
-31.01.2026 firma projeyi hazırlıyor 16.02.2026 tamamlayacak</v>
+        <v xml:space="preserve">Kıymetlendirmede eksiklikler var firma tamamlayacak bu hafta(20.10.2025)
+05.11.2025 eksik uçuşlar teslim edildi
+10.11.2025 kıymetlendirmeler kontrol ediliyor
+13.11.2025 Firmaya 28.11.2025 de teslim edilecek
+15.12.2025 Değerlendirme devam ediyor
+22.12.2025 Kısmi uçuş yapıldı kıymetlendirme yapılıyor aynı zamanda değerlendirme devam ediyor
+02.01.2026 Değerlendirme 15.01.2026 biticek
+31.01.2026 firma projeyi hazırlıyor 16.02.2026 tamamlayacak
+KROKİ/TUTANAK KONTROLLERİ TAMAMLANIP 03.03.2026 İLAN YAPILACAK</v>
       </c>
     </row>
     <row r="116" xml:space="preserve">
@@ -4950,14 +4952,15 @@
         <v>KROKİ/TUTANAK KONTROLÜ</v>
       </c>
       <c r="M116" t="str" xml:space="preserve">
-        <v xml:space="preserve">01.11.2025 firmaya teslim edilecek_x000d_
-05.11.2025 kontroller devam ediyor_x000d_
-13.11.2025 Firmaya 28.11.2025 teslim edilecek_x000d_
-02.12.2025 Firmaya 05.12.2025 teslim edilecek_x000d_
-15.12.2025 Değerlendirme devam ediyor_x000d_
-02.01.2026 Firmaya 15.01.2026 Teslim edilecek_x000d_
-31.01.2026 firma projeyi hazırlıyor 16.02.2026 tamamlayacak_x000d_
-11.02.2026 krokileri firma hazırlıyor</v>
+        <v xml:space="preserve">01.11.2025 firmaya teslim edilecek
+05.11.2025 kontroller devam ediyor
+13.11.2025 Firmaya 28.11.2025 teslim edilecek
+02.12.2025 Firmaya 05.12.2025 teslim edilecek
+15.12.2025 Değerlendirme devam ediyor
+02.01.2026 Firmaya 15.01.2026 Teslim edilecek
+31.01.2026 firma projeyi hazırlıyor 16.02.2026 tamamlayacak
+11.02.2026 krokileri firma hazırlıyor
+KROKİ/TUTANAK KONTROLLERİ 23.02 TAMAMLANIP 03.03.2026 İLAN YAPILACAK</v>
       </c>
     </row>
     <row r="117" xml:space="preserve">
@@ -4998,16 +5001,17 @@
         <v>BİLGİLENDİRME İLANINDA</v>
       </c>
       <c r="M117" t="str" xml:space="preserve">
-        <v xml:space="preserve">01.11.2025 firmaya teslim edilecek_x000d__x000d_
-07.11.2025 firmaya teslim edilecek_x000d__x000d_
-10.11.2025 Firmaya 12.11.2025 de teslim edilecek_x000d__x000d_
-13.11.2025 Firmaya 14.11.2025 de teslim edilecek_x000d__x000d_
-20.11.2025 krokilere 22.11.2025 de başlanarak 24.11.2025 kontrol için verilecek_x000d__x000d_
-02.12.2025 Krokiler hazırlanıp kontrolleri yapılıyor_x000d__x000d_
-15.12.2025 Kroki kontrolü devam ediyor_x000d__x000d_
-22.12.2025 krokiler 24.12.2025 de bitecek_x000d__x000d_
-15.01.2026 Tutanak kontrolü devam ediyor_x000d__x000d_
-31.01.2026 09-13.02 askı ilanı yapılacak</v>
+        <v xml:space="preserve">01.11.2025 firmaya teslim edilecek
+07.11.2025 firmaya teslim edilecek
+10.11.2025 Firmaya 12.11.2025 de teslim edilecek
+13.11.2025 Firmaya 14.11.2025 de teslim edilecek
+20.11.2025 krokilere 22.11.2025 de başlanarak 24.11.2025 kontrol için verilecek
+02.12.2025 Krokiler hazırlanıp kontrolleri yapılıyor
+15.12.2025 Kroki kontrolü devam ediyor
+22.12.2025 krokiler 24.12.2025 de bitecek
+15.01.2026 Tutanak kontrolü devam ediyor
+31.01.2026 09-13.02 askı ilanı yapılacak
+23.02.2026 BİLGİLENDİRME İLANI YAPILACAK</v>
       </c>
     </row>
     <row r="118" xml:space="preserve">
@@ -5048,18 +5052,19 @@
         <v>KROKİ/TUTANAK KONTROLÜ</v>
       </c>
       <c r="M118" t="str" xml:space="preserve">
-        <v xml:space="preserve">01.11.2025 firmaya teslim edilecek_x000d_
-05.11.2025 kontroller devam ediyor_x000d_
-31.01.2026 firma kroki hazırlıyor_x000d_
-10.11.2025 Değerlendrime 13.11.2025 de bitecek_x000d_
-13.11.2025 Firmaya 17-21 haftası teslim edilecek_x000d_
-20.11.2025 firmaya 24.11.2025 de teslim edilecek_x000d_
-02.12.2025 bugün firmaya teslim edilecek_x000d_
-15.12.2025 Proje hazırlanıyor_x000d_
-22.12.2025 Proje 25.12.2025 biticek, krokiler 30.12.2025 verilecek_x000d_
-02.01.2026 Firma projeyi hazırlıyor _x000d_
-15.01.2026 kroki hazırlanıyor_x000d_
-11.02.2026 Kroki kontrolü yapılıyor. Tutanak basılacak 16-20.02 askı</v>
+        <v xml:space="preserve">01.11.2025 firmaya teslim edilecek
+05.11.2025 kontroller devam ediyor
+31.01.2026 firma kroki hazırlıyor
+10.11.2025 Değerlendrime 13.11.2025 de bitecek
+13.11.2025 Firmaya 17-21 haftası teslim edilecek
+20.11.2025 firmaya 24.11.2025 de teslim edilecek
+02.12.2025 bugün firmaya teslim edilecek
+15.12.2025 Proje hazırlanıyor
+22.12.2025 Proje 25.12.2025 biticek, krokiler 30.12.2025 verilecek
+02.01.2026 Firma projeyi hazırlıyor 
+15.01.2026 kroki hazırlanıyor
+11.02.2026 Kroki kontrolü yapılıyor. Tutanak basılacak 16-20.02 askı
+KROKİ/TUTANAK KONTROLLERİ 23.02 TAMAMLANIP 25.02.2026 İLAN YAPILACAK</v>
       </c>
     </row>
     <row r="119" xml:space="preserve">
@@ -5100,9 +5105,10 @@
         <v>FİRMAYA TESLİM EDİLDİ</v>
       </c>
       <c r="M119" t="str" xml:space="preserve">
-        <v xml:space="preserve">15.12.2025 Değerlendirme devam ediyor_x000d__x000d_
-22.12.2025 Arazi uçuş yapılacak yerler var. Değerlendirme devam ediyor._x000d__x000d_
-31.01.2026 Haftaiçi ormancı ve arazi kontrolü sonrası haftasonu firma kroki çalışmalarına başlayacak</v>
+        <v xml:space="preserve">15.12.2025 Değerlendirme devam ediyor
+22.12.2025 Arazi uçuş yapılacak yerler var. Değerlendirme devam ediyor.
+31.01.2026 Haftaiçi ormancı ve arazi kontrolü sonrası haftasonu firma kroki çalışmalarına başlayacak
+KROKİLER BİR KISMI 27.02.2026 TESLİM EDİLECEK. KALAN KISMLAR İLE BİRLİKTE KONTROLLERİ 06.03.2026 YA KADAR TAMAMLANACAK. TUTANAKLAR 10.03 TARİHE KADAR BASILARAK 13.03 KONTROL BİTİCEK.                                                                                                                                                                                                                       16.03.2026 İLAN YAPILACAK</v>
       </c>
     </row>
     <row r="120" xml:space="preserve">
@@ -5143,10 +5149,11 @@
         <v>İHALEDEN/PROGRAMDAN ÇIKARILDI</v>
       </c>
       <c r="M120" t="str" xml:space="preserve">
-        <v xml:space="preserve">14.11.2025 firmaya teslim edilecek_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-12.11.2025 Parsel sayısı OLUR için yazıldı_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-02.12.2025 bu hafta teslim edilecek_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-15.12.2025 GM Rapor hazırlanıyor</v>
+        <v xml:space="preserve">14.11.2025 firmaya teslim edilecek
+12.11.2025 Parsel sayısı OLUR için yazıldı
+02.12.2025 bu hafta teslim edilecek
+15.12.2025 GM Rapor hazırlanıyor
+İHALEDEN ÇIKARILACAK</v>
       </c>
     </row>
     <row r="121" xml:space="preserve">
@@ -5187,14 +5194,15 @@
         <v>BİLGİLENDİRME İLANINDA</v>
       </c>
       <c r="M121" t="str" xml:space="preserve">
-        <v xml:space="preserve">17.10.2025 firmaya teslim edilecek_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-22.10.2025 krokiler basılacak_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-28.10.2025 krokiler basılacak_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-04.11.2025 krokiler basılıp kontrole verildi_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-10.11.2025 Tutanaklar 13.11.2025 imzaya götürülecek_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-13.11.2025 Tutanaklar basılacak_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-20.11.2025 25.11.2025 askıya çıkacak_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-02.12.2025 Askıya çıkacak</v>
+        <v xml:space="preserve">17.10.2025 firmaya teslim edilecek
+22.10.2025 krokiler basılacak
+28.10.2025 krokiler basılacak
+04.11.2025 krokiler basılıp kontrole verildi
+10.11.2025 Tutanaklar 13.11.2025 imzaya götürülecek
+13.11.2025 Tutanaklar basılacak
+20.11.2025 25.11.2025 askıya çıkacak
+02.12.2025 Askıya çıkacak
+KOMİSYON TAMAMLANIP 27.02.2026 KESİN ASKIYA ÇIKACAK</v>
       </c>
     </row>
     <row r="122" xml:space="preserve">
@@ -5235,11 +5243,12 @@
         <v>KOMİSYON AŞAMASINDA</v>
       </c>
       <c r="M122" t="str" xml:space="preserve">
-        <v xml:space="preserve">17.10.2025 Tutanaklara başlanılacak_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-03.11.2025 askı yapılacak(1 bilirkişi eksik nedeniyle)_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-10.11.2025 askıya çıkacak_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-10.11.2025 12.11.2025 askıya çıkacak(Tutanak kontrolü 15.11.2025 de bitip 18.11.2025 askıya çıkacak)_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-20.11.2025 24.11.2025 askıya çıkacak(ormancıda kontrolde bekliyor)</v>
+        <v xml:space="preserve">17.10.2025 Tutanaklara başlanılacak
+03.11.2025 askı yapılacak(1 bilirkişi eksik nedeniyle)
+10.11.2025 askıya çıkacak
+10.11.2025 12.11.2025 askıya çıkacak(Tutanak kontrolü 15.11.2025 de bitip 18.11.2025 askıya çıkacak)
+20.11.2025 24.11.2025 askıya çıkacak(ormancıda kontrolde bekliyor)
+KOMİSYON TAMAMLANIP 25.02.2026 KESİN ASKIYA ÇIKACAK</v>
       </c>
     </row>
     <row r="123">

</xml_diff>

<commit_message>
İş Takip Güncellemesi - 26.02.2026 12:04:50
</commit_message>
<xml_diff>
--- a/istakip.xlsx
+++ b/istakip.xlsx
@@ -4666,7 +4666,7 @@
         <v>2025-05-23</v>
       </c>
       <c r="L110" t="str">
-        <v>BİLGİLENDİRME İLANINDA</v>
+        <v>KESİN ASKIDA</v>
       </c>
       <c r="M110" t="str" xml:space="preserve">
         <v xml:space="preserve">16.10.2025 Taşçılı tutanak Kadastro Üyesine teslim edilecek.
@@ -9308,10 +9308,10 @@
         <v>2025-11-27</v>
       </c>
       <c r="N17" t="str">
-        <v/>
+        <v>Yapıldı</v>
       </c>
       <c r="O17" t="str">
-        <v/>
+        <v>2026-02-27</v>
       </c>
     </row>
     <row r="18">

</xml_diff>

<commit_message>
İş Takip Güncellemesi - 26.02.2026 12:07:21
</commit_message>
<xml_diff>
--- a/istakip.xlsx
+++ b/istakip.xlsx
@@ -4319,7 +4319,7 @@
         <v>2025-05-23</v>
       </c>
       <c r="L102" t="str">
-        <v>KROKİ/TUTANAK KONTROLÜ</v>
+        <v>ASKI İLANINA HAZIRLANIYOR</v>
       </c>
       <c r="M102" t="str" xml:space="preserve">
         <v xml:space="preserve">01.11.2025 firmaya teslim edilecek
@@ -5108,7 +5108,7 @@
         <v xml:space="preserve">15.12.2025 Değerlendirme devam ediyor
 22.12.2025 Arazi uçuş yapılacak yerler var. Değerlendirme devam ediyor.
 31.01.2026 Haftaiçi ormancı ve arazi kontrolü sonrası haftasonu firma kroki çalışmalarına başlayacak
-KROKİLER BİR KISMI 27.02.2026 TESLİM EDİLECEK. KALAN KISMLAR İLE BİRLİKTE KONTROLLERİ 06.03.2026 YA KADAR TAMAMLANACAK. TUTANAKLAR 10.03 TARİHE KADAR BASILARAK 13.03 KONTROL BİTİCEK.                                                                                                                                                                                                                       16.03.2026 İLAN YAPILACAK</v>
+KROKİLER BİR KISMI 27.02.2026 TESLİM EDİLECEK. KALAN KISMLAR İLE BİRLİKTE KONTROLLERİ 06.03.2026 YA KADAR TAMAMLANACAK. TUTANAKLAR 10.03 TARİHE KADAR BASILARAK 13.03 KONTROL BİTİCEK. 16.03.2026 İLAN YAPILACAK</v>
       </c>
     </row>
     <row r="120" xml:space="preserve">

</xml_diff>

<commit_message>
İş Takip Güncellemesi - 27.02.2026 08:21:23
</commit_message>
<xml_diff>
--- a/istakip.xlsx
+++ b/istakip.xlsx
@@ -13676,7 +13676,7 @@
         <v>KIZILÇUKUR</v>
       </c>
       <c r="C13" t="str">
-        <v>MEHMET AKGÜN KOLUKIRIK, İSMAİL AKLAN, LOKMAN ALKAN</v>
+        <v>LOKMAN ALKAN, TAHA GÜRKAN, İSMAİL AKLAN</v>
       </c>
     </row>
     <row r="14">
@@ -13797,7 +13797,7 @@
         <v>BELENKEŞLİK</v>
       </c>
       <c r="C24" t="str">
-        <v>CİHAN KARA, İSMAİL AKLAN, LOKMAN ALKAN</v>
+        <v>İSMAİL PEHLİVAN, CİHAN KARA, İSMAİL AKLAN</v>
       </c>
     </row>
     <row r="25">

</xml_diff>

<commit_message>
İş Takip Güncellemesi - 27.02.2026 09:42:38
</commit_message>
<xml_diff>
--- a/istakip.xlsx
+++ b/istakip.xlsx
@@ -8224,8 +8224,8 @@
         <v>İHALEDEN/PROGRAMDAN ÇIKARILDI</v>
       </c>
       <c r="M200" t="str" xml:space="preserve">
-        <v xml:space="preserve">7139 SK çalışmalarında Bilirkişi seçimi yapıldı. Yemin yaptırılacak._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">7139 SK çalışmalarında Bilirkişi seçimi yapıldı. Yemin yaptırılacak.
+22-a yapılacak
 22-a ihalesine alındı</v>
       </c>
     </row>

</xml_diff>